<commit_message>
modificaciones de los retornos de los TES ppara estimaciones finales
</commit_message>
<xml_diff>
--- a/bases_de_datos/bases_pesonales/base_variables_macro_financieras.xlsx
+++ b/bases_de_datos/bases_pesonales/base_variables_macro_financieras.xlsx
@@ -37,10 +37,10 @@
     <t xml:space="preserve">inflacion_observada</t>
   </si>
   <si>
-    <t xml:space="preserve">tasa_1_año</t>
+    <t xml:space="preserve">tasa_1_año_numero</t>
   </si>
   <si>
-    <t xml:space="preserve">tasa_10_años</t>
+    <t xml:space="preserve">tasa_10_años_numero</t>
   </si>
   <si>
     <t xml:space="preserve">IPI</t>
@@ -171,7 +171,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -180,16 +180,20 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -198,6 +202,10 @@
     </xf>
     <xf numFmtId="166" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -284,15 +292,15 @@
   <dimension ref="A1:H109"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -311,10 +319,10 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -322,7 +330,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
+      <c r="A2" s="3" t="n">
         <v>40544</v>
       </c>
       <c r="B2" s="0" t="n">
@@ -331,24 +339,24 @@
       <c r="C2" s="0" t="n">
         <v>1777.192</v>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="D2" s="2" t="n">
         <v>3.632</v>
       </c>
       <c r="E2" s="4" t="n">
         <v>3.4</v>
       </c>
-      <c r="F2" s="3" t="n">
-        <v>4.42568751046895</v>
-      </c>
-      <c r="G2" s="3" t="n">
-        <v>8.39521236731316</v>
-      </c>
-      <c r="H2" s="5" t="n">
+      <c r="F2" s="5" t="n">
+        <v>0.0442568751046895</v>
+      </c>
+      <c r="G2" s="5" t="n">
+        <v>0.0839521236731316</v>
+      </c>
+      <c r="H2" s="6" t="n">
         <v>132.308205120849</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="n">
+      <c r="A3" s="3" t="n">
         <v>40575</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -357,24 +365,24 @@
       <c r="C3" s="0" t="n">
         <v>1700.5425</v>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="D3" s="2" t="n">
         <v>3.625</v>
       </c>
-      <c r="E3" s="6" t="n">
+      <c r="E3" s="7" t="n">
         <v>3.17</v>
       </c>
-      <c r="F3" s="0" t="n">
-        <v>4.61594379981703</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>8.77614114368595</v>
-      </c>
-      <c r="H3" s="5" t="n">
+      <c r="F3" s="8" t="n">
+        <v>0.0461594379981703</v>
+      </c>
+      <c r="G3" s="8" t="n">
+        <v>0.0877614114368595</v>
+      </c>
+      <c r="H3" s="6" t="n">
         <v>141.147254500039</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
+      <c r="A4" s="3" t="n">
         <v>40603</v>
       </c>
       <c r="B4" s="0" t="n">
@@ -383,24 +391,24 @@
       <c r="C4" s="0" t="n">
         <v>1729.42590909091</v>
       </c>
-      <c r="D4" s="3" t="n">
+      <c r="D4" s="2" t="n">
         <v>3.65</v>
       </c>
       <c r="E4" s="4" t="n">
         <v>3.19</v>
       </c>
-      <c r="F4" s="0" t="n">
-        <v>4.86444236732188</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>8.81959081551339</v>
-      </c>
-      <c r="H4" s="5" t="n">
+      <c r="F4" s="8" t="n">
+        <v>0.0486444236732188</v>
+      </c>
+      <c r="G4" s="8" t="n">
+        <v>0.0881959081551339</v>
+      </c>
+      <c r="H4" s="6" t="n">
         <v>156.311481358133</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="n">
+      <c r="A5" s="3" t="n">
         <v>40634</v>
       </c>
       <c r="B5" s="0" t="n">
@@ -409,24 +417,24 @@
       <c r="C5" s="0" t="n">
         <v>1693.50210526316</v>
       </c>
-      <c r="D5" s="7" t="n">
+      <c r="D5" s="9" t="n">
         <v>3.435</v>
       </c>
-      <c r="E5" s="6" t="n">
+      <c r="E5" s="7" t="n">
         <v>2.84</v>
       </c>
-      <c r="F5" s="0" t="n">
-        <v>4.88691135132096</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>8.54702458272753</v>
-      </c>
-      <c r="H5" s="5" t="n">
+      <c r="F5" s="8" t="n">
+        <v>0.0488691135132096</v>
+      </c>
+      <c r="G5" s="8" t="n">
+        <v>0.0854702458272753</v>
+      </c>
+      <c r="H5" s="6" t="n">
         <v>141.339644493012</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="n">
+      <c r="A6" s="3" t="n">
         <v>40664</v>
       </c>
       <c r="B6" s="0" t="n">
@@ -435,24 +443,24 @@
       <c r="C6" s="0" t="n">
         <v>1702.66272727273</v>
       </c>
-      <c r="D6" s="7" t="n">
+      <c r="D6" s="9" t="n">
         <v>3.5</v>
       </c>
       <c r="E6" s="4" t="n">
         <v>3.02</v>
       </c>
-      <c r="F6" s="0" t="n">
-        <v>5.1499354389031</v>
-      </c>
-      <c r="G6" s="0" t="n">
-        <v>8.41925577982042</v>
-      </c>
-      <c r="H6" s="5" t="n">
+      <c r="F6" s="8" t="n">
+        <v>0.051499354389031</v>
+      </c>
+      <c r="G6" s="8" t="n">
+        <v>0.0841925577982042</v>
+      </c>
+      <c r="H6" s="6" t="n">
         <v>149.698461277321</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="n">
+      <c r="A7" s="3" t="n">
         <v>40695</v>
       </c>
       <c r="B7" s="0" t="n">
@@ -461,24 +469,24 @@
       <c r="C7" s="0" t="n">
         <v>1725.8995</v>
       </c>
-      <c r="D7" s="3" t="n">
+      <c r="D7" s="2" t="n">
         <v>3.5</v>
       </c>
-      <c r="E7" s="6" t="n">
+      <c r="E7" s="7" t="n">
         <v>3.23</v>
       </c>
-      <c r="F7" s="0" t="n">
-        <v>5.23828663499732</v>
-      </c>
-      <c r="G7" s="0" t="n">
-        <v>8.01870743639155</v>
-      </c>
-      <c r="H7" s="5" t="n">
+      <c r="F7" s="8" t="n">
+        <v>0.0523828663499732</v>
+      </c>
+      <c r="G7" s="8" t="n">
+        <v>0.0801870743639155</v>
+      </c>
+      <c r="H7" s="6" t="n">
         <v>142.017374900237</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="n">
+      <c r="A8" s="3" t="n">
         <v>40725</v>
       </c>
       <c r="B8" s="0" t="n">
@@ -487,24 +495,24 @@
       <c r="C8" s="0" t="n">
         <v>1643.81473684211</v>
       </c>
-      <c r="D8" s="7" t="n">
+      <c r="D8" s="9" t="n">
         <v>3.264</v>
       </c>
       <c r="E8" s="4" t="n">
         <v>3.42</v>
       </c>
-      <c r="F8" s="0" t="n">
-        <v>5.27097733154901</v>
-      </c>
-      <c r="G8" s="0" t="n">
-        <v>7.90941296436259</v>
-      </c>
-      <c r="H8" s="5" t="n">
+      <c r="F8" s="8" t="n">
+        <v>0.0527097733154901</v>
+      </c>
+      <c r="G8" s="8" t="n">
+        <v>0.0790941296436259</v>
+      </c>
+      <c r="H8" s="6" t="n">
         <v>149.902921180524</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="n">
+      <c r="A9" s="3" t="n">
         <v>40756</v>
       </c>
       <c r="B9" s="0" t="n">
@@ -513,24 +521,24 @@
       <c r="C9" s="0" t="n">
         <v>1606.96409090909</v>
       </c>
-      <c r="D9" s="7" t="n">
+      <c r="D9" s="9" t="n">
         <v>3.575</v>
       </c>
-      <c r="E9" s="6" t="n">
+      <c r="E9" s="7" t="n">
         <v>3.27</v>
       </c>
-      <c r="F9" s="0" t="n">
-        <v>5.31240493479105</v>
-      </c>
-      <c r="G9" s="0" t="n">
-        <v>7.56235221839032</v>
-      </c>
-      <c r="H9" s="5" t="n">
+      <c r="F9" s="8" t="n">
+        <v>0.0531240493479105</v>
+      </c>
+      <c r="G9" s="8" t="n">
+        <v>0.0756235221839032</v>
+      </c>
+      <c r="H9" s="6" t="n">
         <v>155.204155110813</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="n">
+      <c r="A10" s="3" t="n">
         <v>40787</v>
       </c>
       <c r="B10" s="0" t="n">
@@ -539,24 +547,24 @@
       <c r="C10" s="0" t="n">
         <v>1630.42818181818</v>
       </c>
-      <c r="D10" s="3" t="n">
+      <c r="D10" s="2" t="n">
         <v>3.2</v>
       </c>
       <c r="E10" s="4" t="n">
         <v>3.73</v>
       </c>
-      <c r="F10" s="0" t="n">
-        <v>5.07750937179567</v>
-      </c>
-      <c r="G10" s="0" t="n">
-        <v>7.49014650859139</v>
-      </c>
-      <c r="H10" s="5" t="n">
+      <c r="F10" s="8" t="n">
+        <v>0.0507750937179567</v>
+      </c>
+      <c r="G10" s="8" t="n">
+        <v>0.0749014650859139</v>
+      </c>
+      <c r="H10" s="6" t="n">
         <v>157.502879479768</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="n">
+      <c r="A11" s="3" t="n">
         <v>40817</v>
       </c>
       <c r="B11" s="0" t="n">
@@ -565,24 +573,24 @@
       <c r="C11" s="0" t="n">
         <v>1608.9315</v>
       </c>
-      <c r="D11" s="3" t="n">
+      <c r="D11" s="2" t="n">
         <v>3.622</v>
       </c>
-      <c r="E11" s="6" t="n">
+      <c r="E11" s="7" t="n">
         <v>4.02</v>
       </c>
-      <c r="F11" s="0" t="n">
-        <v>5.3113092338057</v>
-      </c>
-      <c r="G11" s="0" t="n">
-        <v>7.6820407449649</v>
-      </c>
-      <c r="H11" s="5" t="n">
+      <c r="F11" s="8" t="n">
+        <v>0.053113092338057</v>
+      </c>
+      <c r="G11" s="8" t="n">
+        <v>0.076820407449649</v>
+      </c>
+      <c r="H11" s="6" t="n">
         <v>153.161183779447</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="n">
+      <c r="A12" s="3" t="n">
         <v>40848</v>
       </c>
       <c r="B12" s="0" t="n">
@@ -591,24 +599,24 @@
       <c r="C12" s="0" t="n">
         <v>1559.518</v>
       </c>
-      <c r="D12" s="3" t="n">
+      <c r="D12" s="2" t="n">
         <v>3.466</v>
       </c>
       <c r="E12" s="4" t="n">
         <v>3.96</v>
       </c>
-      <c r="F12" s="0" t="n">
-        <v>5.63799567281521</v>
-      </c>
-      <c r="G12" s="0" t="n">
-        <v>7.68277585165647</v>
-      </c>
-      <c r="H12" s="5" t="n">
+      <c r="F12" s="8" t="n">
+        <v>0.0563799567281521</v>
+      </c>
+      <c r="G12" s="8" t="n">
+        <v>0.0768277585165647</v>
+      </c>
+      <c r="H12" s="6" t="n">
         <v>158.805943929004</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="n">
+      <c r="A13" s="3" t="n">
         <v>40878</v>
       </c>
       <c r="B13" s="0" t="n">
@@ -617,24 +625,24 @@
       <c r="C13" s="0" t="n">
         <v>1575.056</v>
       </c>
-      <c r="D13" s="3" t="n">
+      <c r="D13" s="2" t="n">
         <v>3.6</v>
       </c>
-      <c r="E13" s="6" t="n">
+      <c r="E13" s="7" t="n">
         <v>3.73</v>
       </c>
-      <c r="F13" s="0" t="n">
-        <v>5.57447811585682</v>
-      </c>
-      <c r="G13" s="0" t="n">
-        <v>7.75159971907763</v>
-      </c>
-      <c r="H13" s="5" t="n">
+      <c r="F13" s="8" t="n">
+        <v>0.0557447811585682</v>
+      </c>
+      <c r="G13" s="8" t="n">
+        <v>0.0775159971907763</v>
+      </c>
+      <c r="H13" s="6" t="n">
         <v>148.85278413663</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="n">
+      <c r="A14" s="3" t="n">
         <v>40909</v>
       </c>
       <c r="B14" s="0" t="n">
@@ -643,24 +651,24 @@
       <c r="C14" s="0" t="n">
         <v>1603.11857142857</v>
       </c>
-      <c r="D14" s="7" t="n">
+      <c r="D14" s="9" t="n">
         <v>3.538</v>
       </c>
       <c r="E14" s="4" t="n">
         <v>3.54</v>
       </c>
-      <c r="F14" s="0" t="n">
-        <v>5.54226506626396</v>
-      </c>
-      <c r="G14" s="0" t="n">
-        <v>7.57160360664451</v>
-      </c>
-      <c r="H14" s="5" t="n">
+      <c r="F14" s="8" t="n">
+        <v>0.0554226506626396</v>
+      </c>
+      <c r="G14" s="8" t="n">
+        <v>0.0757160360664451</v>
+      </c>
+      <c r="H14" s="6" t="n">
         <v>133.651805758556</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="n">
+      <c r="A15" s="3" t="n">
         <v>40940</v>
       </c>
       <c r="B15" s="0" t="n">
@@ -669,24 +677,24 @@
       <c r="C15" s="0" t="n">
         <v>1681.56142857143</v>
       </c>
-      <c r="D15" s="3" t="n">
+      <c r="D15" s="2" t="n">
         <v>3.35</v>
       </c>
-      <c r="E15" s="6" t="n">
+      <c r="E15" s="7" t="n">
         <v>3.55</v>
       </c>
-      <c r="F15" s="0" t="n">
-        <v>5.64396202633687</v>
-      </c>
-      <c r="G15" s="0" t="n">
-        <v>7.48061333456256</v>
-      </c>
-      <c r="H15" s="5" t="n">
+      <c r="F15" s="8" t="n">
+        <v>0.0564396202633687</v>
+      </c>
+      <c r="G15" s="8" t="n">
+        <v>0.0748061333456256</v>
+      </c>
+      <c r="H15" s="6" t="n">
         <v>146.683757856777</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="n">
+      <c r="A16" s="3" t="n">
         <v>40969</v>
       </c>
       <c r="B16" s="0" t="n">
@@ -695,24 +703,24 @@
       <c r="C16" s="0" t="n">
         <v>1729.48857142857</v>
       </c>
-      <c r="D16" s="3" t="n">
+      <c r="D16" s="2" t="n">
         <v>3.5</v>
       </c>
       <c r="E16" s="4" t="n">
         <v>3.4</v>
       </c>
-      <c r="F16" s="0" t="n">
-        <v>5.68881953688457</v>
-      </c>
-      <c r="G16" s="0" t="n">
-        <v>7.38124041341566</v>
-      </c>
-      <c r="H16" s="5" t="n">
+      <c r="F16" s="8" t="n">
+        <v>0.0568881953688457</v>
+      </c>
+      <c r="G16" s="8" t="n">
+        <v>0.0738124041341566</v>
+      </c>
+      <c r="H16" s="6" t="n">
         <v>154.833471950542</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="n">
+      <c r="A17" s="3" t="n">
         <v>41000</v>
       </c>
       <c r="B17" s="0" t="n">
@@ -721,24 +729,24 @@
       <c r="C17" s="0" t="n">
         <v>1753.22666666667</v>
       </c>
-      <c r="D17" s="7" t="n">
+      <c r="D17" s="9" t="n">
         <v>3.497</v>
       </c>
-      <c r="E17" s="6" t="n">
+      <c r="E17" s="7" t="n">
         <v>3.43</v>
       </c>
-      <c r="F17" s="0" t="n">
-        <v>5.501850182229</v>
-      </c>
-      <c r="G17" s="0" t="n">
-        <v>7.24495843572903</v>
-      </c>
-      <c r="H17" s="5" t="n">
+      <c r="F17" s="8" t="n">
+        <v>0.05501850182229</v>
+      </c>
+      <c r="G17" s="8" t="n">
+        <v>0.0724495843572903</v>
+      </c>
+      <c r="H17" s="6" t="n">
         <v>137.273937278388</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="n">
+      <c r="A18" s="3" t="n">
         <v>41030</v>
       </c>
       <c r="B18" s="0" t="n">
@@ -747,24 +755,24 @@
       <c r="C18" s="0" t="n">
         <v>1749.18904761905</v>
       </c>
-      <c r="D18" s="3" t="n">
+      <c r="D18" s="2" t="n">
         <v>3.35</v>
       </c>
       <c r="E18" s="4" t="n">
         <v>3.44</v>
       </c>
-      <c r="F18" s="0" t="n">
-        <v>5.54684006892077</v>
-      </c>
-      <c r="G18" s="0" t="n">
-        <v>7.22107602696059</v>
-      </c>
-      <c r="H18" s="5" t="n">
+      <c r="F18" s="8" t="n">
+        <v>0.0554684006892077</v>
+      </c>
+      <c r="G18" s="8" t="n">
+        <v>0.0722107602696059</v>
+      </c>
+      <c r="H18" s="6" t="n">
         <v>150.302137230029</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="n">
+      <c r="A19" s="3" t="n">
         <v>41061</v>
       </c>
       <c r="B19" s="0" t="n">
@@ -773,24 +781,24 @@
       <c r="C19" s="0" t="n">
         <v>1650.22368421053</v>
       </c>
-      <c r="D19" s="3" t="n">
+      <c r="D19" s="2" t="n">
         <v>3.5</v>
       </c>
-      <c r="E19" s="6" t="n">
+      <c r="E19" s="7" t="n">
         <v>3.2</v>
       </c>
-      <c r="F19" s="0" t="n">
-        <v>5.54497896258604</v>
-      </c>
-      <c r="G19" s="0" t="n">
-        <v>7.15150128515395</v>
-      </c>
-      <c r="H19" s="5" t="n">
+      <c r="F19" s="8" t="n">
+        <v>0.0554497896258604</v>
+      </c>
+      <c r="G19" s="8" t="n">
+        <v>0.0715150128515395</v>
+      </c>
+      <c r="H19" s="6" t="n">
         <v>146.272011034403</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="n">
+      <c r="A20" s="3" t="n">
         <v>41091</v>
       </c>
       <c r="B20" s="0" t="n">
@@ -799,24 +807,24 @@
       <c r="C20" s="0" t="n">
         <v>1663.1995</v>
       </c>
-      <c r="D20" s="3" t="n">
+      <c r="D20" s="2" t="n">
         <v>3.219</v>
       </c>
       <c r="E20" s="4" t="n">
         <v>3.03</v>
       </c>
-      <c r="F20" s="0" t="n">
-        <v>5.44131473628791</v>
-      </c>
-      <c r="G20" s="0" t="n">
-        <v>6.92569977689177</v>
-      </c>
-      <c r="H20" s="5" t="n">
+      <c r="F20" s="8" t="n">
+        <v>0.0544131473628791</v>
+      </c>
+      <c r="G20" s="8" t="n">
+        <v>0.0692569977689177</v>
+      </c>
+      <c r="H20" s="6" t="n">
         <v>153.320601954092</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="n">
+      <c r="A21" s="3" t="n">
         <v>41122</v>
       </c>
       <c r="B21" s="0" t="n">
@@ -825,24 +833,24 @@
       <c r="C21" s="0" t="n">
         <v>1665.54285714286</v>
       </c>
-      <c r="D21" s="3" t="n">
+      <c r="D21" s="2" t="n">
         <v>3.175</v>
       </c>
-      <c r="E21" s="6" t="n">
+      <c r="E21" s="7" t="n">
         <v>3.11</v>
       </c>
-      <c r="F21" s="0" t="n">
-        <v>4.98265933711788</v>
-      </c>
-      <c r="G21" s="0" t="n">
-        <v>6.72848160224395</v>
-      </c>
-      <c r="H21" s="5" t="n">
+      <c r="F21" s="8" t="n">
+        <v>0.0498265933711788</v>
+      </c>
+      <c r="G21" s="8" t="n">
+        <v>0.0672848160224395</v>
+      </c>
+      <c r="H21" s="6" t="n">
         <v>151.735100843701</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="n">
+      <c r="A22" s="3" t="n">
         <v>41153</v>
       </c>
       <c r="B22" s="0" t="n">
@@ -851,24 +859,24 @@
       <c r="C22" s="0" t="n">
         <v>1685.62285714286</v>
       </c>
-      <c r="D22" s="3" t="n">
+      <c r="D22" s="2" t="n">
         <v>3.2</v>
       </c>
       <c r="E22" s="4" t="n">
         <v>3.08</v>
       </c>
-      <c r="F22" s="0" t="n">
-        <v>4.79166609528281</v>
-      </c>
-      <c r="G22" s="0" t="n">
-        <v>6.6203750240593</v>
-      </c>
-      <c r="H22" s="5" t="n">
+      <c r="F22" s="8" t="n">
+        <v>0.0479166609528281</v>
+      </c>
+      <c r="G22" s="8" t="n">
+        <v>0.066203750240593</v>
+      </c>
+      <c r="H22" s="6" t="n">
         <v>155.052972210691</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="n">
+      <c r="A23" s="3" t="n">
         <v>41183</v>
       </c>
       <c r="B23" s="0" t="n">
@@ -877,24 +885,24 @@
       <c r="C23" s="0" t="n">
         <v>1750.755</v>
       </c>
-      <c r="D23" s="3" t="n">
+      <c r="D23" s="2" t="n">
         <v>3.503</v>
       </c>
-      <c r="E23" s="6" t="n">
+      <c r="E23" s="7" t="n">
         <v>3.06</v>
       </c>
-      <c r="F23" s="0" t="n">
-        <v>4.82989059554273</v>
-      </c>
-      <c r="G23" s="0" t="n">
-        <v>6.18996040798258</v>
-      </c>
-      <c r="H23" s="5" t="n">
+      <c r="F23" s="8" t="n">
+        <v>0.0482989059554273</v>
+      </c>
+      <c r="G23" s="8" t="n">
+        <v>0.0618996040798258</v>
+      </c>
+      <c r="H23" s="6" t="n">
         <v>154.701820640583</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="n">
+      <c r="A24" s="3" t="n">
         <v>41214</v>
       </c>
       <c r="B24" s="0" t="n">
@@ -903,24 +911,24 @@
       <c r="C24" s="0" t="n">
         <v>1742.863</v>
       </c>
-      <c r="D24" s="3" t="n">
+      <c r="D24" s="2" t="n">
         <v>2.975</v>
       </c>
       <c r="E24" s="4" t="n">
         <v>2.77</v>
       </c>
-      <c r="F24" s="0" t="n">
-        <v>5.02329099351601</v>
-      </c>
-      <c r="G24" s="0" t="n">
-        <v>6.20219816716478</v>
-      </c>
-      <c r="H24" s="5" t="n">
+      <c r="F24" s="8" t="n">
+        <v>0.0502329099351601</v>
+      </c>
+      <c r="G24" s="8" t="n">
+        <v>0.0620219816716478</v>
+      </c>
+      <c r="H24" s="6" t="n">
         <v>151.948316010846</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="n">
+      <c r="A25" s="3" t="n">
         <v>41244</v>
       </c>
       <c r="B25" s="0" t="n">
@@ -929,24 +937,24 @@
       <c r="C25" s="0" t="n">
         <v>1809.09210526316</v>
       </c>
-      <c r="D25" s="3" t="n">
+      <c r="D25" s="2" t="n">
         <v>3.44</v>
       </c>
-      <c r="E25" s="6" t="n">
+      <c r="E25" s="7" t="n">
         <v>2.44</v>
       </c>
-      <c r="F25" s="0" t="n">
-        <v>4.78237041306818</v>
-      </c>
-      <c r="G25" s="0" t="n">
-        <v>5.90491165129296</v>
-      </c>
-      <c r="H25" s="5" t="n">
+      <c r="F25" s="8" t="n">
+        <v>0.0478237041306818</v>
+      </c>
+      <c r="G25" s="8" t="n">
+        <v>0.0590491165129296</v>
+      </c>
+      <c r="H25" s="6" t="n">
         <v>144.431356397159</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="n">
+      <c r="A26" s="3" t="n">
         <v>41275</v>
       </c>
       <c r="B26" s="0" t="n">
@@ -955,24 +963,24 @@
       <c r="C26" s="0" t="n">
         <v>1847.354</v>
       </c>
-      <c r="D26" s="3" t="n">
+      <c r="D26" s="2" t="n">
         <v>3.365</v>
       </c>
       <c r="E26" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="F26" s="0" t="n">
-        <v>4.30895746838593</v>
-      </c>
-      <c r="G26" s="0" t="n">
-        <v>5.46354965507105</v>
-      </c>
-      <c r="H26" s="5" t="n">
+      <c r="F26" s="8" t="n">
+        <v>0.0430895746838593</v>
+      </c>
+      <c r="G26" s="8" t="n">
+        <v>0.0546354965507105</v>
+      </c>
+      <c r="H26" s="6" t="n">
         <v>133.101813468134</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="n">
+      <c r="A27" s="3" t="n">
         <v>41306</v>
       </c>
       <c r="B27" s="0" t="n">
@@ -981,24 +989,24 @@
       <c r="C27" s="0" t="n">
         <v>1861.7575</v>
       </c>
-      <c r="D27" s="3" t="n">
+      <c r="D27" s="2" t="n">
         <v>3.3</v>
       </c>
-      <c r="E27" s="6" t="n">
+      <c r="E27" s="7" t="n">
         <v>1.83</v>
       </c>
-      <c r="F27" s="0" t="n">
-        <v>4.15727880320796</v>
-      </c>
-      <c r="G27" s="0" t="n">
-        <v>5.15245082934611</v>
-      </c>
-      <c r="H27" s="5" t="n">
+      <c r="F27" s="8" t="n">
+        <v>0.0415727880320796</v>
+      </c>
+      <c r="G27" s="8" t="n">
+        <v>0.0515245082934611</v>
+      </c>
+      <c r="H27" s="6" t="n">
         <v>139.564322354181</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="n">
+      <c r="A28" s="3" t="n">
         <v>41334</v>
       </c>
       <c r="B28" s="0" t="n">
@@ -1007,24 +1015,24 @@
       <c r="C28" s="0" t="n">
         <v>1790.7</v>
       </c>
-      <c r="D28" s="3" t="n">
+      <c r="D28" s="2" t="n">
         <v>3.4</v>
       </c>
       <c r="E28" s="4" t="n">
         <v>1.91</v>
       </c>
-      <c r="F28" s="0" t="n">
-        <v>3.86622092427687</v>
-      </c>
-      <c r="G28" s="0" t="n">
-        <v>5.07509879594376</v>
-      </c>
-      <c r="H28" s="5" t="n">
+      <c r="F28" s="8" t="n">
+        <v>0.0386622092427687</v>
+      </c>
+      <c r="G28" s="8" t="n">
+        <v>0.0507509879594376</v>
+      </c>
+      <c r="H28" s="6" t="n">
         <v>136.843705109732</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2" t="n">
+      <c r="A29" s="3" t="n">
         <v>41365</v>
       </c>
       <c r="B29" s="0" t="n">
@@ -1033,24 +1041,24 @@
       <c r="C29" s="0" t="n">
         <v>1725.48590909091</v>
       </c>
-      <c r="D29" s="3" t="n">
+      <c r="D29" s="2" t="n">
         <v>3.311</v>
       </c>
-      <c r="E29" s="6" t="n">
+      <c r="E29" s="7" t="n">
         <v>2.02</v>
       </c>
-      <c r="F29" s="0" t="n">
-        <v>3.63325159184527</v>
-      </c>
-      <c r="G29" s="0" t="n">
-        <v>5.15973485505166</v>
-      </c>
-      <c r="H29" s="5" t="n">
+      <c r="F29" s="8" t="n">
+        <v>0.0363325159184527</v>
+      </c>
+      <c r="G29" s="8" t="n">
+        <v>0.0515973485505166</v>
+      </c>
+      <c r="H29" s="6" t="n">
         <v>149.989432506216</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="n">
+      <c r="A30" s="3" t="n">
         <v>41395</v>
       </c>
       <c r="B30" s="0" t="n">
@@ -1059,24 +1067,24 @@
       <c r="C30" s="0" t="n">
         <v>1688.53619047619</v>
       </c>
-      <c r="D30" s="3" t="n">
+      <c r="D30" s="2" t="n">
         <v>3.2</v>
       </c>
       <c r="E30" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="F30" s="0" t="n">
-        <v>3.90556689883275</v>
-      </c>
-      <c r="G30" s="0" t="n">
-        <v>5.42641934968032</v>
-      </c>
-      <c r="H30" s="5" t="n">
+      <c r="F30" s="8" t="n">
+        <v>0.0390556689883275</v>
+      </c>
+      <c r="G30" s="8" t="n">
+        <v>0.0542641934968032</v>
+      </c>
+      <c r="H30" s="6" t="n">
         <v>147.324756920101</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="n">
+      <c r="A31" s="3" t="n">
         <v>41426</v>
       </c>
       <c r="B31" s="0" t="n">
@@ -1085,24 +1093,24 @@
       <c r="C31" s="0" t="n">
         <v>1628.56722222222</v>
       </c>
-      <c r="D31" s="3" t="n">
+      <c r="D31" s="2" t="n">
         <v>3.3</v>
       </c>
-      <c r="E31" s="6" t="n">
+      <c r="E31" s="7" t="n">
         <v>2.16</v>
       </c>
-      <c r="F31" s="0" t="n">
-        <v>4.2778800267863</v>
-      </c>
-      <c r="G31" s="0" t="n">
-        <v>6.98136853853739</v>
-      </c>
-      <c r="H31" s="5" t="n">
+      <c r="F31" s="8" t="n">
+        <v>0.042778800267863</v>
+      </c>
+      <c r="G31" s="8" t="n">
+        <v>0.0698136853853739</v>
+      </c>
+      <c r="H31" s="6" t="n">
         <v>138.908835468829</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="n">
+      <c r="A32" s="3" t="n">
         <v>41456</v>
       </c>
       <c r="B32" s="0" t="n">
@@ -1111,24 +1119,24 @@
       <c r="C32" s="0" t="n">
         <v>1643.98772727273</v>
       </c>
-      <c r="D32" s="7" t="n">
+      <c r="D32" s="9" t="n">
         <v>3.239</v>
       </c>
       <c r="E32" s="4" t="n">
         <v>2.22</v>
       </c>
-      <c r="F32" s="0" t="n">
-        <v>4.29531957681601</v>
-      </c>
-      <c r="G32" s="0" t="n">
-        <v>7.15128701549697</v>
-      </c>
-      <c r="H32" s="5" t="n">
+      <c r="F32" s="8" t="n">
+        <v>0.0429531957681601</v>
+      </c>
+      <c r="G32" s="8" t="n">
+        <v>0.0715128701549697</v>
+      </c>
+      <c r="H32" s="6" t="n">
         <v>154.871904401688</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="2" t="n">
+      <c r="A33" s="3" t="n">
         <v>41487</v>
       </c>
       <c r="B33" s="0" t="n">
@@ -1137,24 +1145,24 @@
       <c r="C33" s="0" t="n">
         <v>1723.694</v>
       </c>
-      <c r="D33" s="3" t="n">
+      <c r="D33" s="2" t="n">
         <v>3.05</v>
       </c>
-      <c r="E33" s="6" t="n">
+      <c r="E33" s="7" t="n">
         <v>2.27</v>
       </c>
-      <c r="F33" s="0" t="n">
-        <v>4.43003993802434</v>
-      </c>
-      <c r="G33" s="0" t="n">
-        <v>7.57946853536899</v>
-      </c>
-      <c r="H33" s="5" t="n">
+      <c r="F33" s="8" t="n">
+        <v>0.0443003993802434</v>
+      </c>
+      <c r="G33" s="8" t="n">
+        <v>0.0757946853536899</v>
+      </c>
+      <c r="H33" s="6" t="n">
         <v>147.389690264538</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="2" t="n">
+      <c r="A34" s="3" t="n">
         <v>41518</v>
       </c>
       <c r="B34" s="0" t="n">
@@ -1163,24 +1171,24 @@
       <c r="C34" s="0" t="n">
         <v>1759.80285714286</v>
       </c>
-      <c r="D34" s="3" t="n">
+      <c r="D34" s="2" t="n">
         <v>3.15</v>
       </c>
       <c r="E34" s="4" t="n">
         <v>2.27</v>
       </c>
-      <c r="F34" s="0" t="n">
-        <v>4.28221778292483</v>
-      </c>
-      <c r="G34" s="0" t="n">
-        <v>7.51209140485462</v>
-      </c>
-      <c r="H34" s="5" t="n">
+      <c r="F34" s="8" t="n">
+        <v>0.0428221778292483</v>
+      </c>
+      <c r="G34" s="8" t="n">
+        <v>0.0751209140485462</v>
+      </c>
+      <c r="H34" s="6" t="n">
         <v>156.621802832485</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="2" t="n">
+      <c r="A35" s="3" t="n">
         <v>41548</v>
       </c>
       <c r="B35" s="0" t="n">
@@ -1189,24 +1197,24 @@
       <c r="C35" s="0" t="n">
         <v>1763.34818181818</v>
       </c>
-      <c r="D35" s="3" t="n">
+      <c r="D35" s="2" t="n">
         <v>2.856</v>
       </c>
-      <c r="E35" s="6" t="n">
+      <c r="E35" s="7" t="n">
         <v>1.84</v>
       </c>
-      <c r="F35" s="0" t="n">
-        <v>4.18953197581603</v>
-      </c>
-      <c r="G35" s="0" t="n">
-        <v>7.08182953008537</v>
-      </c>
-      <c r="H35" s="5" t="n">
+      <c r="F35" s="8" t="n">
+        <v>0.0418953197581603</v>
+      </c>
+      <c r="G35" s="8" t="n">
+        <v>0.0708182953008537</v>
+      </c>
+      <c r="H35" s="6" t="n">
         <v>155.965639165483</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="2" t="n">
+      <c r="A36" s="3" t="n">
         <v>41579</v>
       </c>
       <c r="B36" s="0" t="n">
@@ -1215,24 +1223,24 @@
       <c r="C36" s="0" t="n">
         <v>1668.71368421053</v>
       </c>
-      <c r="D36" s="3" t="n">
+      <c r="D36" s="2" t="n">
         <v>2.875</v>
       </c>
       <c r="E36" s="4" t="n">
         <v>1.76</v>
       </c>
-      <c r="F36" s="0" t="n">
-        <v>4.22743085223348</v>
-      </c>
-      <c r="G36" s="0" t="n">
-        <v>7.34533347195988</v>
-      </c>
-      <c r="H36" s="5" t="n">
+      <c r="F36" s="8" t="n">
+        <v>0.0422743085223348</v>
+      </c>
+      <c r="G36" s="8" t="n">
+        <v>0.0734533347195988</v>
+      </c>
+      <c r="H36" s="6" t="n">
         <v>152.113707839208</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="2" t="n">
+      <c r="A37" s="3" t="n">
         <v>41609</v>
       </c>
       <c r="B37" s="0" t="n">
@@ -1241,24 +1249,24 @@
       <c r="C37" s="0" t="n">
         <v>1614.644</v>
       </c>
-      <c r="D37" s="3" t="n">
+      <c r="D37" s="2" t="n">
         <v>2.86</v>
       </c>
-      <c r="E37" s="6" t="n">
+      <c r="E37" s="7" t="n">
         <v>1.94</v>
       </c>
-      <c r="F37" s="0" t="n">
-        <v>4.20301563903005</v>
-      </c>
-      <c r="G37" s="0" t="n">
-        <v>7.27106247837205</v>
-      </c>
-      <c r="H37" s="5" t="n">
+      <c r="F37" s="8" t="n">
+        <v>0.0420301563903005</v>
+      </c>
+      <c r="G37" s="8" t="n">
+        <v>0.0727106247837205</v>
+      </c>
+      <c r="H37" s="6" t="n">
         <v>147.359035474977</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="2" t="n">
+      <c r="A38" s="3" t="n">
         <v>41640</v>
       </c>
       <c r="B38" s="0" t="n">
@@ -1267,24 +1275,24 @@
       <c r="C38" s="0" t="n">
         <v>1527.93571428571</v>
       </c>
-      <c r="D38" s="3" t="n">
+      <c r="D38" s="2" t="n">
         <v>3.15</v>
       </c>
       <c r="E38" s="4" t="n">
         <v>2.13</v>
       </c>
-      <c r="F38" s="0" t="n">
-        <v>4.16082026234887</v>
-      </c>
-      <c r="G38" s="0" t="n">
-        <v>7.32995153246596</v>
-      </c>
-      <c r="H38" s="5" t="n">
+      <c r="F38" s="8" t="n">
+        <v>0.0416082026234887</v>
+      </c>
+      <c r="G38" s="8" t="n">
+        <v>0.0732995153246596</v>
+      </c>
+      <c r="H38" s="6" t="n">
         <v>134.390893286124</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="2" t="n">
+      <c r="A39" s="3" t="n">
         <v>41671</v>
       </c>
       <c r="B39" s="0" t="n">
@@ -1293,24 +1301,24 @@
       <c r="C39" s="0" t="n">
         <v>1504.55</v>
       </c>
-      <c r="D39" s="3" t="n">
+      <c r="D39" s="2" t="n">
         <v>3.025</v>
       </c>
-      <c r="E39" s="6" t="n">
+      <c r="E39" s="7" t="n">
         <v>2.32</v>
       </c>
-      <c r="F39" s="0" t="n">
-        <v>4.30858091373125</v>
-      </c>
-      <c r="G39" s="0" t="n">
-        <v>7.60728855343778</v>
-      </c>
-      <c r="H39" s="5" t="n">
+      <c r="F39" s="8" t="n">
+        <v>0.0430858091373125</v>
+      </c>
+      <c r="G39" s="8" t="n">
+        <v>0.0760728855343778</v>
+      </c>
+      <c r="H39" s="6" t="n">
         <v>145.491844684106</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="2" t="n">
+      <c r="A40" s="3" t="n">
         <v>41699</v>
       </c>
       <c r="B40" s="0" t="n">
@@ -1319,24 +1327,24 @@
       <c r="C40" s="0" t="n">
         <v>1600.4985</v>
       </c>
-      <c r="D40" s="3" t="n">
+      <c r="D40" s="2" t="n">
         <v>3.1</v>
       </c>
       <c r="E40" s="4" t="n">
         <v>2.51</v>
       </c>
-      <c r="F40" s="0" t="n">
-        <v>4.14341075848751</v>
-      </c>
-      <c r="G40" s="0" t="n">
-        <v>7.39868838177599</v>
-      </c>
-      <c r="H40" s="5" t="n">
+      <c r="F40" s="8" t="n">
+        <v>0.0414341075848751</v>
+      </c>
+      <c r="G40" s="8" t="n">
+        <v>0.0739868838177599</v>
+      </c>
+      <c r="H40" s="6" t="n">
         <v>149.949395748444</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="2" t="n">
+      <c r="A41" s="3" t="n">
         <v>41730</v>
       </c>
       <c r="B41" s="0" t="n">
@@ -1345,24 +1353,24 @@
       <c r="C41" s="0" t="n">
         <v>1672.556</v>
       </c>
-      <c r="D41" s="3" t="n">
+      <c r="D41" s="2" t="n">
         <v>3.201</v>
       </c>
-      <c r="E41" s="6" t="n">
+      <c r="E41" s="7" t="n">
         <v>2.72</v>
       </c>
-      <c r="F41" s="0" t="n">
-        <v>4.22344296295047</v>
-      </c>
-      <c r="G41" s="0" t="n">
-        <v>6.61569164543857</v>
-      </c>
-      <c r="H41" s="5" t="n">
+      <c r="F41" s="8" t="n">
+        <v>0.0422344296295047</v>
+      </c>
+      <c r="G41" s="8" t="n">
+        <v>0.0661569164543857</v>
+      </c>
+      <c r="H41" s="6" t="n">
         <v>164.354105692507</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="2" t="n">
+      <c r="A42" s="3" t="n">
         <v>41760</v>
       </c>
       <c r="B42" s="0" t="n">
@@ -1371,24 +1379,24 @@
       <c r="C42" s="0" t="n">
         <v>1669.62952380952</v>
       </c>
-      <c r="D42" s="3" t="n">
+      <c r="D42" s="2" t="n">
         <v>3.025</v>
       </c>
       <c r="E42" s="4" t="n">
         <v>2.93</v>
       </c>
-      <c r="F42" s="0" t="n">
-        <v>4.4958681077554</v>
-      </c>
-      <c r="G42" s="0" t="n">
-        <v>6.63380662004808</v>
-      </c>
-      <c r="H42" s="5" t="n">
+      <c r="F42" s="8" t="n">
+        <v>0.044958681077554</v>
+      </c>
+      <c r="G42" s="8" t="n">
+        <v>0.0663380662004808</v>
+      </c>
+      <c r="H42" s="6" t="n">
         <v>149.909820482992</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="2" t="n">
+      <c r="A43" s="3" t="n">
         <v>41791</v>
       </c>
       <c r="B43" s="0" t="n">
@@ -1397,24 +1405,24 @@
       <c r="C43" s="0" t="n">
         <v>1707.61055555556</v>
       </c>
-      <c r="D43" s="3" t="n">
+      <c r="D43" s="2" t="n">
         <v>3.15</v>
       </c>
-      <c r="E43" s="6" t="n">
+      <c r="E43" s="7" t="n">
         <v>2.79</v>
       </c>
-      <c r="F43" s="0" t="n">
-        <v>4.69978114468524</v>
-      </c>
-      <c r="G43" s="0" t="n">
-        <v>6.75429326472703</v>
-      </c>
-      <c r="H43" s="5" t="n">
+      <c r="F43" s="8" t="n">
+        <v>0.0469978114468524</v>
+      </c>
+      <c r="G43" s="8" t="n">
+        <v>0.0675429326472703</v>
+      </c>
+      <c r="H43" s="6" t="n">
         <v>138.542278162285</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="2" t="n">
+      <c r="A44" s="3" t="n">
         <v>41821</v>
       </c>
       <c r="B44" s="0" t="n">
@@ -1423,24 +1431,24 @@
       <c r="C44" s="0" t="n">
         <v>1694.83391304348</v>
       </c>
-      <c r="D44" s="3" t="n">
+      <c r="D44" s="2" t="n">
         <v>3.11</v>
       </c>
       <c r="E44" s="4" t="n">
         <v>2.89</v>
       </c>
-      <c r="F44" s="0" t="n">
-        <v>4.74129773741143</v>
-      </c>
-      <c r="G44" s="0" t="n">
-        <v>6.88551983635803</v>
-      </c>
-      <c r="H44" s="5" t="n">
+      <c r="F44" s="8" t="n">
+        <v>0.0474129773741143</v>
+      </c>
+      <c r="G44" s="8" t="n">
+        <v>0.0688551983635803</v>
+      </c>
+      <c r="H44" s="6" t="n">
         <v>157.731760583727</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="2" t="n">
+      <c r="A45" s="3" t="n">
         <v>41852</v>
       </c>
       <c r="B45" s="0" t="n">
@@ -1449,24 +1457,24 @@
       <c r="C45" s="0" t="n">
         <v>1736.39421052632</v>
       </c>
-      <c r="D45" s="3" t="n">
+      <c r="D45" s="2" t="n">
         <v>3.125</v>
       </c>
-      <c r="E45" s="6" t="n">
+      <c r="E45" s="7" t="n">
         <v>3.02</v>
       </c>
-      <c r="F45" s="0" t="n">
-        <v>4.79345034189505</v>
-      </c>
-      <c r="G45" s="0" t="n">
-        <v>6.95068215793488</v>
-      </c>
-      <c r="H45" s="5" t="n">
+      <c r="F45" s="8" t="n">
+        <v>0.0479345034189505</v>
+      </c>
+      <c r="G45" s="8" t="n">
+        <v>0.0695068215793488</v>
+      </c>
+      <c r="H45" s="6" t="n">
         <v>147.793736048353</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="2" t="n">
+      <c r="A46" s="3" t="n">
         <v>41883</v>
       </c>
       <c r="B46" s="0" t="n">
@@ -1475,24 +1483,24 @@
       <c r="C46" s="0" t="n">
         <v>1729.995</v>
       </c>
-      <c r="D46" s="3" t="n">
+      <c r="D46" s="2" t="n">
         <v>3.12</v>
       </c>
       <c r="E46" s="4" t="n">
         <v>2.86</v>
       </c>
-      <c r="F46" s="0" t="n">
-        <v>4.85273664127318</v>
-      </c>
-      <c r="G46" s="0" t="n">
-        <v>6.91040121773688</v>
-      </c>
-      <c r="H46" s="5" t="n">
+      <c r="F46" s="8" t="n">
+        <v>0.0485273664127318</v>
+      </c>
+      <c r="G46" s="8" t="n">
+        <v>0.0691040121773688</v>
+      </c>
+      <c r="H46" s="6" t="n">
         <v>159.513972543982</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="2" t="n">
+      <c r="A47" s="3" t="n">
         <v>41913</v>
       </c>
       <c r="B47" s="0" t="n">
@@ -1501,24 +1509,24 @@
       <c r="C47" s="0" t="n">
         <v>1623.66636363636</v>
       </c>
-      <c r="D47" s="3" t="n">
+      <c r="D47" s="2" t="n">
         <v>2.967</v>
       </c>
-      <c r="E47" s="6" t="n">
+      <c r="E47" s="7" t="n">
         <v>3.29</v>
       </c>
-      <c r="F47" s="0" t="n">
-        <v>4.87193305807499</v>
-      </c>
-      <c r="G47" s="0" t="n">
-        <v>7.01255125288507</v>
-      </c>
-      <c r="H47" s="5" t="n">
+      <c r="F47" s="8" t="n">
+        <v>0.0487193305807499</v>
+      </c>
+      <c r="G47" s="8" t="n">
+        <v>0.0701255125288507</v>
+      </c>
+      <c r="H47" s="6" t="n">
         <v>156.22704927792</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="2" t="n">
+      <c r="A48" s="3" t="n">
         <v>41944</v>
       </c>
       <c r="B48" s="0" t="n">
@@ -1527,24 +1535,24 @@
       <c r="C48" s="0" t="n">
         <v>1598.36722222222</v>
       </c>
-      <c r="D48" s="3" t="n">
+      <c r="D48" s="2" t="n">
         <v>3.05</v>
       </c>
       <c r="E48" s="4" t="n">
         <v>3.65</v>
       </c>
-      <c r="F48" s="0" t="n">
-        <v>4.79012678607116</v>
-      </c>
-      <c r="G48" s="0" t="n">
-        <v>6.84668485365683</v>
-      </c>
-      <c r="H48" s="5" t="n">
+      <c r="F48" s="8" t="n">
+        <v>0.0479012678607116</v>
+      </c>
+      <c r="G48" s="8" t="n">
+        <v>0.0684668485365683</v>
+      </c>
+      <c r="H48" s="6" t="n">
         <v>150.378681860094</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="2" t="n">
+      <c r="A49" s="3" t="n">
         <v>41974</v>
       </c>
       <c r="B49" s="0" t="n">
@@ -1553,24 +1561,24 @@
       <c r="C49" s="0" t="n">
         <v>1471.5225</v>
       </c>
-      <c r="D49" s="3" t="n">
+      <c r="D49" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="E49" s="6" t="n">
+      <c r="E49" s="7" t="n">
         <v>3.66</v>
       </c>
-      <c r="F49" s="0" t="n">
-        <v>4.81628795860605</v>
-      </c>
-      <c r="G49" s="0" t="n">
-        <v>7.39200345448761</v>
-      </c>
-      <c r="H49" s="5" t="n">
+      <c r="F49" s="8" t="n">
+        <v>0.0481628795860605</v>
+      </c>
+      <c r="G49" s="8" t="n">
+        <v>0.0739200345448761</v>
+      </c>
+      <c r="H49" s="6" t="n">
         <v>150.553221195364</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="2" t="n">
+      <c r="A50" s="3" t="n">
         <v>42005</v>
       </c>
       <c r="B50" s="0" t="n">
@@ -1579,24 +1587,24 @@
       <c r="C50" s="0" t="n">
         <v>1409.6685</v>
       </c>
-      <c r="D50" s="3" t="n">
+      <c r="D50" s="2" t="n">
         <v>3.219</v>
       </c>
       <c r="E50" s="4" t="n">
         <v>3.82</v>
       </c>
-      <c r="F50" s="0" t="n">
-        <v>4.71815625859054</v>
-      </c>
-      <c r="G50" s="0" t="n">
-        <v>7.12724221438546</v>
-      </c>
-      <c r="H50" s="5" t="n">
+      <c r="F50" s="8" t="n">
+        <v>0.0471815625859054</v>
+      </c>
+      <c r="G50" s="8" t="n">
+        <v>0.0712724221438546</v>
+      </c>
+      <c r="H50" s="6" t="n">
         <v>131.505406805762</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="2" t="n">
+      <c r="A51" s="3" t="n">
         <v>42036</v>
       </c>
       <c r="B51" s="0" t="n">
@@ -1605,24 +1613,24 @@
       <c r="C51" s="0" t="n">
         <v>1395.8375</v>
       </c>
-      <c r="D51" s="3" t="n">
+      <c r="D51" s="2" t="n">
         <v>3.3</v>
       </c>
-      <c r="E51" s="6" t="n">
+      <c r="E51" s="7" t="n">
         <v>4.36</v>
       </c>
-      <c r="F51" s="0" t="n">
-        <v>4.62181545065299</v>
-      </c>
-      <c r="G51" s="0" t="n">
-        <v>7.0273018933916</v>
-      </c>
-      <c r="H51" s="5" t="n">
+      <c r="F51" s="8" t="n">
+        <v>0.0462181545065299</v>
+      </c>
+      <c r="G51" s="8" t="n">
+        <v>0.070273018933916</v>
+      </c>
+      <c r="H51" s="6" t="n">
         <v>145.853805475076</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="2" t="n">
+      <c r="A52" s="3" t="n">
         <v>42064</v>
       </c>
       <c r="B52" s="0" t="n">
@@ -1631,24 +1639,24 @@
       <c r="C52" s="0" t="n">
         <v>1292.09333333333</v>
       </c>
-      <c r="D52" s="3" t="n">
+      <c r="D52" s="2" t="n">
         <v>3.25</v>
       </c>
       <c r="E52" s="4" t="n">
         <v>4.56</v>
       </c>
-      <c r="F52" s="0" t="n">
-        <v>4.78510869782394</v>
-      </c>
-      <c r="G52" s="0" t="n">
-        <v>7.31796594694353</v>
-      </c>
-      <c r="H52" s="5" t="n">
+      <c r="F52" s="8" t="n">
+        <v>0.0478510869782394</v>
+      </c>
+      <c r="G52" s="8" t="n">
+        <v>0.0731796594694353</v>
+      </c>
+      <c r="H52" s="6" t="n">
         <v>151.874735652948</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="2" t="n">
+      <c r="A53" s="3" t="n">
         <v>42095</v>
       </c>
       <c r="B53" s="0" t="n">
@@ -1657,24 +1665,24 @@
       <c r="C53" s="0" t="n">
         <v>1362.6075</v>
       </c>
-      <c r="D53" s="3" t="n">
+      <c r="D53" s="2" t="n">
         <v>3.243</v>
       </c>
-      <c r="E53" s="6" t="n">
+      <c r="E53" s="7" t="n">
         <v>4.64</v>
       </c>
-      <c r="F53" s="0" t="n">
-        <v>4.73559756494373</v>
-      </c>
-      <c r="G53" s="0" t="n">
-        <v>7.20813907841762</v>
-      </c>
-      <c r="H53" s="5" t="n">
+      <c r="F53" s="8" t="n">
+        <v>0.0473559756494373</v>
+      </c>
+      <c r="G53" s="8" t="n">
+        <v>0.0720813907841762</v>
+      </c>
+      <c r="H53" s="6" t="n">
         <v>162.204641344745</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="2" t="n">
+      <c r="A54" s="3" t="n">
         <v>42125</v>
       </c>
       <c r="B54" s="0" t="n">
@@ -1683,24 +1691,24 @@
       <c r="C54" s="0" t="n">
         <v>1359.53684210526</v>
       </c>
-      <c r="D54" s="3" t="n">
+      <c r="D54" s="2" t="n">
         <v>3.25</v>
       </c>
       <c r="E54" s="4" t="n">
         <v>4.41</v>
       </c>
-      <c r="F54" s="0" t="n">
-        <v>4.71361618524128</v>
-      </c>
-      <c r="G54" s="0" t="n">
-        <v>7.35220513932068</v>
-      </c>
-      <c r="H54" s="5" t="n">
+      <c r="F54" s="8" t="n">
+        <v>0.0471361618524128</v>
+      </c>
+      <c r="G54" s="8" t="n">
+        <v>0.0735220513932068</v>
+      </c>
+      <c r="H54" s="6" t="n">
         <v>147.721923979359</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="2" t="n">
+      <c r="A55" s="3" t="n">
         <v>42156</v>
       </c>
       <c r="B55" s="0" t="n">
@@ -1709,24 +1717,24 @@
       <c r="C55" s="0" t="n">
         <v>1319.74947368421</v>
       </c>
-      <c r="D55" s="3" t="n">
+      <c r="D55" s="2" t="n">
         <v>3.2</v>
       </c>
-      <c r="E55" s="6" t="n">
+      <c r="E55" s="7" t="n">
         <v>4.42</v>
       </c>
-      <c r="F55" s="0" t="n">
-        <v>4.63487916001713</v>
-      </c>
-      <c r="G55" s="0" t="n">
-        <v>7.62272263846286</v>
-      </c>
-      <c r="H55" s="5" t="n">
+      <c r="F55" s="8" t="n">
+        <v>0.0463487916001713</v>
+      </c>
+      <c r="G55" s="8" t="n">
+        <v>0.0762272263846286</v>
+      </c>
+      <c r="H55" s="6" t="n">
         <v>145.445576035509</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="2" t="n">
+      <c r="A56" s="3" t="n">
         <v>42186</v>
       </c>
       <c r="B56" s="0" t="n">
@@ -1735,24 +1743,24 @@
       <c r="C56" s="0" t="n">
         <v>1310.95454545455</v>
       </c>
-      <c r="D56" s="3" t="n">
+      <c r="D56" s="2" t="n">
         <v>3.232</v>
       </c>
       <c r="E56" s="4" t="n">
         <v>4.46</v>
       </c>
-      <c r="F56" s="0" t="n">
-        <v>4.62700842888496</v>
-      </c>
-      <c r="G56" s="0" t="n">
-        <v>7.83985476107019</v>
-      </c>
-      <c r="H56" s="5" t="n">
+      <c r="F56" s="8" t="n">
+        <v>0.0462700842888496</v>
+      </c>
+      <c r="G56" s="8" t="n">
+        <v>0.0783985476107019</v>
+      </c>
+      <c r="H56" s="6" t="n">
         <v>159.897102424764</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="2" t="n">
+      <c r="A57" s="3" t="n">
         <v>42217</v>
       </c>
       <c r="B57" s="0" t="n">
@@ -1761,24 +1769,24 @@
       <c r="C57" s="0" t="n">
         <v>1241.84210526316</v>
       </c>
-      <c r="D57" s="3" t="n">
+      <c r="D57" s="2" t="n">
         <v>3.05</v>
       </c>
-      <c r="E57" s="6" t="n">
+      <c r="E57" s="7" t="n">
         <v>4.74</v>
       </c>
-      <c r="F57" s="0" t="n">
-        <v>5.05412019359837</v>
-      </c>
-      <c r="G57" s="0" t="n">
-        <v>8.05920257237027</v>
-      </c>
-      <c r="H57" s="5" t="n">
+      <c r="F57" s="8" t="n">
+        <v>0.0505412019359837</v>
+      </c>
+      <c r="G57" s="8" t="n">
+        <v>0.0805920257237027</v>
+      </c>
+      <c r="H57" s="6" t="n">
         <v>153.023835041839</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="2" t="n">
+      <c r="A58" s="3" t="n">
         <v>42248</v>
       </c>
       <c r="B58" s="0" t="n">
@@ -1787,24 +1795,24 @@
       <c r="C58" s="0" t="n">
         <v>1233.11863636364</v>
       </c>
-      <c r="D58" s="3" t="n">
+      <c r="D58" s="2" t="n">
         <v>3.1</v>
       </c>
       <c r="E58" s="4" t="n">
         <v>5.35</v>
       </c>
-      <c r="F58" s="0" t="n">
-        <v>5.31958669752539</v>
-      </c>
-      <c r="G58" s="0" t="n">
-        <v>8.59154244741492</v>
-      </c>
-      <c r="H58" s="5" t="n">
+      <c r="F58" s="8" t="n">
+        <v>0.0531958669752539</v>
+      </c>
+      <c r="G58" s="8" t="n">
+        <v>0.0859154244741492</v>
+      </c>
+      <c r="H58" s="6" t="n">
         <v>164.506188524143</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="2" t="n">
+      <c r="A59" s="3" t="n">
         <v>42278</v>
       </c>
       <c r="B59" s="0" t="n">
@@ -1813,24 +1821,24 @@
       <c r="C59" s="0" t="n">
         <v>1246.69238095238</v>
       </c>
-      <c r="D59" s="3" t="n">
+      <c r="D59" s="2" t="n">
         <v>3.14</v>
       </c>
-      <c r="E59" s="6" t="n">
+      <c r="E59" s="7" t="n">
         <v>5.89</v>
       </c>
-      <c r="F59" s="0" t="n">
-        <v>5.54135414442748</v>
-      </c>
-      <c r="G59" s="0" t="n">
-        <v>8.22260473160217</v>
-      </c>
-      <c r="H59" s="5" t="n">
+      <c r="F59" s="8" t="n">
+        <v>0.0554135414442748</v>
+      </c>
+      <c r="G59" s="8" t="n">
+        <v>0.0822260473160217</v>
+      </c>
+      <c r="H59" s="6" t="n">
         <v>160.206672563418</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="2" t="n">
+      <c r="A60" s="3" t="n">
         <v>42309</v>
       </c>
       <c r="B60" s="0" t="n">
@@ -1839,24 +1847,24 @@
       <c r="C60" s="0" t="n">
         <v>1159.84421052632</v>
       </c>
-      <c r="D60" s="3" t="n">
+      <c r="D60" s="2" t="n">
         <v>3.4</v>
       </c>
       <c r="E60" s="4" t="n">
         <v>6.39</v>
       </c>
-      <c r="F60" s="0" t="n">
-        <v>5.97731699900786</v>
-      </c>
-      <c r="G60" s="0" t="n">
-        <v>8.5444233569413</v>
-      </c>
-      <c r="H60" s="5" t="n">
+      <c r="F60" s="8" t="n">
+        <v>0.0597731699900786</v>
+      </c>
+      <c r="G60" s="8" t="n">
+        <v>0.085444233569413</v>
+      </c>
+      <c r="H60" s="6" t="n">
         <v>161.109497736503</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="2" t="n">
+      <c r="A61" s="3" t="n">
         <v>42339</v>
       </c>
       <c r="B61" s="0" t="n">
@@ -1865,24 +1873,24 @@
       <c r="C61" s="0" t="n">
         <v>1111.868</v>
       </c>
-      <c r="D61" s="3" t="n">
+      <c r="D61" s="2" t="n">
         <v>3.3</v>
       </c>
-      <c r="E61" s="6" t="n">
+      <c r="E61" s="7" t="n">
         <v>6.77</v>
       </c>
-      <c r="F61" s="0" t="n">
-        <v>6.4163609886635</v>
-      </c>
-      <c r="G61" s="0" t="n">
-        <v>8.87273707689881</v>
-      </c>
-      <c r="H61" s="5" t="n">
+      <c r="F61" s="8" t="n">
+        <v>0.064163609886635</v>
+      </c>
+      <c r="G61" s="8" t="n">
+        <v>0.0887273707689881</v>
+      </c>
+      <c r="H61" s="6" t="n">
         <v>157.412359417211</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="2" t="n">
+      <c r="A62" s="3" t="n">
         <v>42370</v>
       </c>
       <c r="B62" s="0" t="n">
@@ -1891,24 +1899,24 @@
       <c r="C62" s="0" t="n">
         <v>1124.08894736842</v>
       </c>
-      <c r="D62" s="3" t="n">
+      <c r="D62" s="2" t="n">
         <v>3.138</v>
       </c>
       <c r="E62" s="4" t="n">
         <v>7.45</v>
       </c>
-      <c r="F62" s="0" t="n">
-        <v>6.60377591950287</v>
-      </c>
-      <c r="G62" s="0" t="n">
-        <v>9.15757605946165</v>
-      </c>
-      <c r="H62" s="5" t="n">
+      <c r="F62" s="8" t="n">
+        <v>0.0660377591950287</v>
+      </c>
+      <c r="G62" s="8" t="n">
+        <v>0.0915757605946165</v>
+      </c>
+      <c r="H62" s="6" t="n">
         <v>141.82127294395</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="2" t="n">
+      <c r="A63" s="3" t="n">
         <v>42401</v>
       </c>
       <c r="B63" s="0" t="n">
@@ -1917,24 +1925,24 @@
       <c r="C63" s="0" t="n">
         <v>1211.81095238095</v>
       </c>
-      <c r="D63" s="3" t="n">
+      <c r="D63" s="2" t="n">
         <v>2.825</v>
       </c>
-      <c r="E63" s="6" t="n">
+      <c r="E63" s="7" t="n">
         <v>7.59</v>
       </c>
-      <c r="F63" s="0" t="n">
-        <v>6.79439604718283</v>
-      </c>
-      <c r="G63" s="0" t="n">
-        <v>9.3488826708759</v>
-      </c>
-      <c r="H63" s="5" t="n">
+      <c r="F63" s="8" t="n">
+        <v>0.0679439604718283</v>
+      </c>
+      <c r="G63" s="8" t="n">
+        <v>0.093488826708759</v>
+      </c>
+      <c r="H63" s="6" t="n">
         <v>155.173375783565</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="2" t="n">
+      <c r="A64" s="3" t="n">
         <v>42430</v>
       </c>
       <c r="B64" s="0" t="n">
@@ -1943,24 +1951,24 @@
       <c r="C64" s="0" t="n">
         <v>1299.784</v>
       </c>
-      <c r="D64" s="3" t="n">
+      <c r="D64" s="2" t="n">
         <v>3</v>
       </c>
       <c r="E64" s="4" t="n">
         <v>7.98</v>
       </c>
-      <c r="F64" s="0" t="n">
-        <v>6.79550037084334</v>
-      </c>
-      <c r="G64" s="0" t="n">
-        <v>8.69283351392284</v>
-      </c>
-      <c r="H64" s="5" t="n">
+      <c r="F64" s="8" t="n">
+        <v>0.0679550037084334</v>
+      </c>
+      <c r="G64" s="8" t="n">
+        <v>0.0869283351392284</v>
+      </c>
+      <c r="H64" s="6" t="n">
         <v>152.893010807766</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="2" t="n">
+      <c r="A65" s="3" t="n">
         <v>42461</v>
       </c>
       <c r="B65" s="0" t="n">
@@ -1969,24 +1977,24 @@
       <c r="C65" s="0" t="n">
         <v>1351.20523809524</v>
       </c>
-      <c r="D65" s="3" t="n">
+      <c r="D65" s="2" t="n">
         <v>3.038</v>
       </c>
-      <c r="E65" s="6" t="n">
+      <c r="E65" s="7" t="n">
         <v>7.93</v>
       </c>
-      <c r="F65" s="0" t="n">
-        <v>7.08187090560285</v>
-      </c>
-      <c r="G65" s="0" t="n">
-        <v>8.26994087050675</v>
-      </c>
-      <c r="H65" s="5" t="n">
+      <c r="F65" s="8" t="n">
+        <v>0.0708187090560285</v>
+      </c>
+      <c r="G65" s="8" t="n">
+        <v>0.0826994087050675</v>
+      </c>
+      <c r="H65" s="6" t="n">
         <v>177.029685573313</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="2" t="n">
+      <c r="A66" s="3" t="n">
         <v>42491</v>
       </c>
       <c r="B66" s="0" t="n">
@@ -1995,24 +2003,24 @@
       <c r="C66" s="0" t="n">
         <v>1322.4335</v>
       </c>
-      <c r="D66" s="3" t="n">
+      <c r="D66" s="2" t="n">
         <v>3.1</v>
       </c>
       <c r="E66" s="4" t="n">
         <v>8.2</v>
       </c>
-      <c r="F66" s="0" t="n">
-        <v>7.20352123154181</v>
-      </c>
-      <c r="G66" s="0" t="n">
-        <v>8.19298730105966</v>
-      </c>
-      <c r="H66" s="5" t="n">
+      <c r="F66" s="8" t="n">
+        <v>0.0720352123154181</v>
+      </c>
+      <c r="G66" s="8" t="n">
+        <v>0.0819298730105966</v>
+      </c>
+      <c r="H66" s="6" t="n">
         <v>155.474551253538</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="2" t="n">
+      <c r="A67" s="3" t="n">
         <v>42522</v>
       </c>
       <c r="B67" s="0" t="n">
@@ -2021,24 +2029,24 @@
       <c r="C67" s="0" t="n">
         <v>1314.17238095238</v>
       </c>
-      <c r="D67" s="3" t="n">
+      <c r="D67" s="2" t="n">
         <v>3.05</v>
       </c>
-      <c r="E67" s="6" t="n">
+      <c r="E67" s="7" t="n">
         <v>8.6</v>
       </c>
-      <c r="F67" s="0" t="n">
-        <v>7.03761797609418</v>
-      </c>
-      <c r="G67" s="0" t="n">
-        <v>7.97370889721013</v>
-      </c>
-      <c r="H67" s="5" t="n">
+      <c r="F67" s="8" t="n">
+        <v>0.0703761797609418</v>
+      </c>
+      <c r="G67" s="8" t="n">
+        <v>0.0797370889721013</v>
+      </c>
+      <c r="H67" s="6" t="n">
         <v>155.101610714128</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="2" t="n">
+      <c r="A68" s="3" t="n">
         <v>42552</v>
       </c>
       <c r="B68" s="0" t="n">
@@ -2047,24 +2055,24 @@
       <c r="C68" s="0" t="n">
         <v>1319.77947368421</v>
       </c>
-      <c r="D68" s="3" t="n">
+      <c r="D68" s="2" t="n">
         <v>3.678</v>
       </c>
       <c r="E68" s="4" t="n">
         <v>8.97</v>
       </c>
-      <c r="F68" s="0" t="n">
-        <v>6.91407922413266</v>
-      </c>
-      <c r="G68" s="0" t="n">
-        <v>7.60060383681652</v>
-      </c>
-      <c r="H68" s="5" t="n">
+      <c r="F68" s="8" t="n">
+        <v>0.0691407922413266</v>
+      </c>
+      <c r="G68" s="8" t="n">
+        <v>0.0760060383681652</v>
+      </c>
+      <c r="H68" s="6" t="n">
         <v>150.078556949137</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="2" t="n">
+      <c r="A69" s="3" t="n">
         <v>42583</v>
       </c>
       <c r="B69" s="0" t="n">
@@ -2073,24 +2081,24 @@
       <c r="C69" s="0" t="n">
         <v>1340.015</v>
       </c>
-      <c r="D69" s="3" t="n">
+      <c r="D69" s="2" t="n">
         <v>3.5</v>
       </c>
-      <c r="E69" s="6" t="n">
+      <c r="E69" s="7" t="n">
         <v>8.1</v>
       </c>
-      <c r="F69" s="0" t="n">
-        <v>7.22365266854504</v>
-      </c>
-      <c r="G69" s="0" t="n">
-        <v>7.49581596223608</v>
-      </c>
-      <c r="H69" s="5" t="n">
+      <c r="F69" s="8" t="n">
+        <v>0.0722365266854504</v>
+      </c>
+      <c r="G69" s="8" t="n">
+        <v>0.0749581596223608</v>
+      </c>
+      <c r="H69" s="6" t="n">
         <v>168.76299202311</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="2" t="n">
+      <c r="A70" s="3" t="n">
         <v>42614</v>
       </c>
       <c r="B70" s="0" t="n">
@@ -2099,24 +2107,24 @@
       <c r="C70" s="0" t="n">
         <v>1369.43863636364</v>
       </c>
-      <c r="D70" s="3" t="n">
+      <c r="D70" s="2" t="n">
         <v>3.6</v>
       </c>
       <c r="E70" s="4" t="n">
         <v>7.27</v>
       </c>
-      <c r="F70" s="0" t="n">
-        <v>6.92160603267282</v>
-      </c>
-      <c r="G70" s="0" t="n">
-        <v>7.15751475398952</v>
-      </c>
-      <c r="H70" s="5" t="n">
+      <c r="F70" s="8" t="n">
+        <v>0.0692160603267282</v>
+      </c>
+      <c r="G70" s="8" t="n">
+        <v>0.0715751475398952</v>
+      </c>
+      <c r="H70" s="6" t="n">
         <v>172.135673249435</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="2" t="n">
+      <c r="A71" s="3" t="n">
         <v>42644</v>
       </c>
       <c r="B71" s="0" t="n">
@@ -2125,24 +2133,24 @@
       <c r="C71" s="0" t="n">
         <v>1353.292</v>
       </c>
-      <c r="D71" s="3" t="n">
+      <c r="D71" s="2" t="n">
         <v>3.46</v>
       </c>
-      <c r="E71" s="6" t="n">
+      <c r="E71" s="7" t="n">
         <v>6.48</v>
       </c>
-      <c r="F71" s="0" t="n">
-        <v>6.85381107879448</v>
-      </c>
-      <c r="G71" s="0" t="n">
-        <v>7.23201660580738</v>
-      </c>
-      <c r="H71" s="5" t="n">
+      <c r="F71" s="8" t="n">
+        <v>0.0685381107879448</v>
+      </c>
+      <c r="G71" s="8" t="n">
+        <v>0.0723201660580738</v>
+      </c>
+      <c r="H71" s="6" t="n">
         <v>161.075164063552</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="2" t="n">
+      <c r="A72" s="3" t="n">
         <v>42675</v>
       </c>
       <c r="B72" s="0" t="n">
@@ -2151,24 +2159,24 @@
       <c r="C72" s="0" t="n">
         <v>1318.006</v>
       </c>
-      <c r="D72" s="3" t="n">
+      <c r="D72" s="2" t="n">
         <v>3.275</v>
       </c>
       <c r="E72" s="4" t="n">
         <v>5.96</v>
       </c>
-      <c r="F72" s="0" t="n">
-        <v>6.98392480745571</v>
-      </c>
-      <c r="G72" s="0" t="n">
-        <v>7.53580336388032</v>
-      </c>
-      <c r="H72" s="5" t="n">
+      <c r="F72" s="8" t="n">
+        <v>0.0698392480745571</v>
+      </c>
+      <c r="G72" s="8" t="n">
+        <v>0.0753580336388032</v>
+      </c>
+      <c r="H72" s="6" t="n">
         <v>164.499379216581</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="2" t="n">
+      <c r="A73" s="3" t="n">
         <v>42705</v>
       </c>
       <c r="B73" s="0" t="n">
@@ -2177,24 +2185,24 @@
       <c r="C73" s="0" t="n">
         <v>1331.24</v>
       </c>
-      <c r="D73" s="3" t="n">
+      <c r="D73" s="2" t="n">
         <v>3.35</v>
       </c>
-      <c r="E73" s="6" t="n">
+      <c r="E73" s="7" t="n">
         <v>5.75</v>
       </c>
-      <c r="F73" s="0" t="n">
-        <v>6.80617033998848</v>
-      </c>
-      <c r="G73" s="0" t="n">
-        <v>7.34978307548942</v>
-      </c>
-      <c r="H73" s="5" t="n">
+      <c r="F73" s="8" t="n">
+        <v>0.0680617033998848</v>
+      </c>
+      <c r="G73" s="8" t="n">
+        <v>0.0734978307548942</v>
+      </c>
+      <c r="H73" s="6" t="n">
         <v>162.084756467353</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="2" t="n">
+      <c r="A74" s="3" t="n">
         <v>42736</v>
       </c>
       <c r="B74" s="0" t="n">
@@ -2203,24 +2211,24 @@
       <c r="C74" s="0" t="n">
         <v>1364.93095238095</v>
       </c>
-      <c r="D74" s="3" t="n">
+      <c r="D74" s="2" t="n">
         <v>3.73</v>
       </c>
       <c r="E74" s="4" t="n">
         <v>5.47</v>
       </c>
-      <c r="F74" s="0" t="n">
-        <v>6.45484048969393</v>
-      </c>
-      <c r="G74" s="0" t="n">
-        <v>6.95450330595559</v>
-      </c>
-      <c r="H74" s="5" t="n">
+      <c r="F74" s="8" t="n">
+        <v>0.0645484048969393</v>
+      </c>
+      <c r="G74" s="8" t="n">
+        <v>0.0695450330595559</v>
+      </c>
+      <c r="H74" s="6" t="n">
         <v>142.667566713108</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="2" t="n">
+      <c r="A75" s="3" t="n">
         <v>42767</v>
       </c>
       <c r="B75" s="0" t="n">
@@ -2229,24 +2237,24 @@
       <c r="C75" s="0" t="n">
         <v>1345.2405</v>
       </c>
-      <c r="D75" s="3" t="n">
+      <c r="D75" s="2" t="n">
         <v>3.92</v>
       </c>
-      <c r="E75" s="6" t="n">
+      <c r="E75" s="7" t="n">
         <v>5.18</v>
       </c>
-      <c r="F75" s="0" t="n">
-        <v>6.60979434414998</v>
-      </c>
-      <c r="G75" s="0" t="n">
-        <v>6.91545934978313</v>
-      </c>
-      <c r="H75" s="5" t="n">
+      <c r="F75" s="8" t="n">
+        <v>0.0660979434414998</v>
+      </c>
+      <c r="G75" s="8" t="n">
+        <v>0.0691545934978313</v>
+      </c>
+      <c r="H75" s="6" t="n">
         <v>151.184023689116</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="2" t="n">
+      <c r="A76" s="3" t="n">
         <v>42795</v>
       </c>
       <c r="B76" s="0" t="n">
@@ -2255,24 +2263,24 @@
       <c r="C76" s="0" t="n">
         <v>1342.81090909091</v>
       </c>
-      <c r="D76" s="3" t="n">
+      <c r="D76" s="2" t="n">
         <v>3.81</v>
       </c>
       <c r="E76" s="4" t="n">
         <v>4.69</v>
       </c>
-      <c r="F76" s="0" t="n">
-        <v>6.35241715427773</v>
-      </c>
-      <c r="G76" s="0" t="n">
-        <v>6.99390032236706</v>
-      </c>
-      <c r="H76" s="5" t="n">
+      <c r="F76" s="8" t="n">
+        <v>0.0635241715427773</v>
+      </c>
+      <c r="G76" s="8" t="n">
+        <v>0.0699390032236706</v>
+      </c>
+      <c r="H76" s="6" t="n">
         <v>160.713598378572</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="2" t="n">
+      <c r="A77" s="3" t="n">
         <v>42826</v>
       </c>
       <c r="B77" s="0" t="n">
@@ -2281,24 +2289,24 @@
       <c r="C77" s="0" t="n">
         <v>1369.77833333333</v>
       </c>
-      <c r="D77" s="3" t="n">
+      <c r="D77" s="2" t="n">
         <v>3.833</v>
       </c>
-      <c r="E77" s="6" t="n">
+      <c r="E77" s="7" t="n">
         <v>4.66</v>
       </c>
-      <c r="F77" s="0" t="n">
-        <v>5.96535628724215</v>
-      </c>
-      <c r="G77" s="0" t="n">
-        <v>6.63282345832022</v>
-      </c>
-      <c r="H77" s="5" t="n">
+      <c r="F77" s="8" t="n">
+        <v>0.0596535628724215</v>
+      </c>
+      <c r="G77" s="8" t="n">
+        <v>0.0663282345832022</v>
+      </c>
+      <c r="H77" s="6" t="n">
         <v>164.180257154474</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="2" t="n">
+      <c r="A78" s="3" t="n">
         <v>42856</v>
       </c>
       <c r="B78" s="0" t="n">
@@ -2307,24 +2315,24 @@
       <c r="C78" s="0" t="n">
         <v>1424.3019047619</v>
       </c>
-      <c r="D78" s="3" t="n">
+      <c r="D78" s="2" t="n">
         <v>4.361</v>
       </c>
       <c r="E78" s="4" t="n">
         <v>4.37</v>
       </c>
-      <c r="F78" s="0" t="n">
-        <v>5.57557046993958</v>
-      </c>
-      <c r="G78" s="0" t="n">
-        <v>6.49725220030844</v>
-      </c>
-      <c r="H78" s="5" t="n">
+      <c r="F78" s="8" t="n">
+        <v>0.0557557046993958</v>
+      </c>
+      <c r="G78" s="8" t="n">
+        <v>0.0649725220030844</v>
+      </c>
+      <c r="H78" s="6" t="n">
         <v>155.092197261535</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="2" t="n">
+      <c r="A79" s="3" t="n">
         <v>42887</v>
       </c>
       <c r="B79" s="0" t="n">
@@ -2333,24 +2341,24 @@
       <c r="C79" s="0" t="n">
         <v>1449.015</v>
       </c>
-      <c r="D79" s="3" t="n">
+      <c r="D79" s="2" t="n">
         <v>3.7</v>
       </c>
-      <c r="E79" s="6" t="n">
+      <c r="E79" s="7" t="n">
         <v>3.99</v>
       </c>
-      <c r="F79" s="0" t="n">
-        <v>5.15617531404117</v>
-      </c>
-      <c r="G79" s="0" t="n">
-        <v>6.52846688425177</v>
-      </c>
-      <c r="H79" s="5" t="n">
+      <c r="F79" s="8" t="n">
+        <v>0.0515617531404117</v>
+      </c>
+      <c r="G79" s="8" t="n">
+        <v>0.0652846688425177</v>
+      </c>
+      <c r="H79" s="6" t="n">
         <v>153.140141579467</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="2" t="n">
+      <c r="A80" s="3" t="n">
         <v>42917</v>
       </c>
       <c r="B80" s="0" t="n">
@@ -2359,24 +2367,24 @@
       <c r="C80" s="0" t="n">
         <v>1478.95894736842</v>
       </c>
-      <c r="D80" s="3" t="n">
+      <c r="D80" s="2" t="n">
         <v>4.341</v>
       </c>
       <c r="E80" s="4" t="n">
         <v>3.4</v>
       </c>
-      <c r="F80" s="0" t="n">
-        <v>5.30449124696687</v>
-      </c>
-      <c r="G80" s="0" t="n">
-        <v>6.96311558152952</v>
-      </c>
-      <c r="H80" s="5" t="n">
+      <c r="F80" s="8" t="n">
+        <v>0.0530449124696687</v>
+      </c>
+      <c r="G80" s="8" t="n">
+        <v>0.0696311558152952</v>
+      </c>
+      <c r="H80" s="6" t="n">
         <v>160.381952918095</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="2" t="n">
+      <c r="A81" s="3" t="n">
         <v>42948</v>
       </c>
       <c r="B81" s="0" t="n">
@@ -2385,24 +2393,24 @@
       <c r="C81" s="0" t="n">
         <v>1473.11476190476</v>
       </c>
-      <c r="D81" s="3" t="n">
+      <c r="D81" s="2" t="n">
         <v>4.066</v>
       </c>
-      <c r="E81" s="6" t="n">
+      <c r="E81" s="7" t="n">
         <v>3.87</v>
       </c>
-      <c r="F81" s="0" t="n">
-        <v>5.39843638716445</v>
-      </c>
-      <c r="G81" s="0" t="n">
-        <v>6.98365914324625</v>
-      </c>
-      <c r="H81" s="5" t="n">
+      <c r="F81" s="8" t="n">
+        <v>0.0539843638716445</v>
+      </c>
+      <c r="G81" s="8" t="n">
+        <v>0.0698365914324625</v>
+      </c>
+      <c r="H81" s="6" t="n">
         <v>164.147680910857</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="2" t="n">
+      <c r="A82" s="3" t="n">
         <v>42979</v>
       </c>
       <c r="B82" s="0" t="n">
@@ -2411,24 +2419,24 @@
       <c r="C82" s="0" t="n">
         <v>1493.37142857143</v>
       </c>
-      <c r="D82" s="3" t="n">
+      <c r="D82" s="2" t="n">
         <v>4.2</v>
       </c>
       <c r="E82" s="4" t="n">
         <v>3.97</v>
       </c>
-      <c r="F82" s="0" t="n">
-        <v>5.1502986324976</v>
-      </c>
-      <c r="G82" s="0" t="n">
-        <v>6.7968119329004</v>
-      </c>
-      <c r="H82" s="5" t="n">
+      <c r="F82" s="8" t="n">
+        <v>0.051502986324976</v>
+      </c>
+      <c r="G82" s="8" t="n">
+        <v>0.067968119329004</v>
+      </c>
+      <c r="H82" s="6" t="n">
         <v>168.308369038778</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="2" t="n">
+      <c r="A83" s="3" t="n">
         <v>43009</v>
       </c>
       <c r="B83" s="0" t="n">
@@ -2437,24 +2445,24 @@
       <c r="C83" s="0" t="n">
         <v>1472.61428571429</v>
       </c>
-      <c r="D83" s="3" t="n">
+      <c r="D83" s="2" t="n">
         <v>4.33</v>
       </c>
-      <c r="E83" s="6" t="n">
+      <c r="E83" s="7" t="n">
         <v>4.05</v>
       </c>
-      <c r="F83" s="0" t="n">
-        <v>5.12998488486601</v>
-      </c>
-      <c r="G83" s="0" t="n">
-        <v>6.72678820600958</v>
-      </c>
-      <c r="H83" s="5" t="n">
+      <c r="F83" s="8" t="n">
+        <v>0.0512998488486601</v>
+      </c>
+      <c r="G83" s="8" t="n">
+        <v>0.0672678820600958</v>
+      </c>
+      <c r="H83" s="6" t="n">
         <v>160.689587243547</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="2" t="n">
+      <c r="A84" s="3" t="n">
         <v>43040</v>
       </c>
       <c r="B84" s="0" t="n">
@@ -2463,24 +2471,24 @@
       <c r="C84" s="0" t="n">
         <v>1439.9855</v>
       </c>
-      <c r="D84" s="3" t="n">
+      <c r="D84" s="2" t="n">
         <v>4.61</v>
       </c>
       <c r="E84" s="4" t="n">
         <v>4.12</v>
       </c>
-      <c r="F84" s="0" t="n">
-        <v>4.87911232903806</v>
-      </c>
-      <c r="G84" s="0" t="n">
-        <v>6.88760909635338</v>
-      </c>
-      <c r="H84" s="5" t="n">
+      <c r="F84" s="8" t="n">
+        <v>0.0487911232903806</v>
+      </c>
+      <c r="G84" s="8" t="n">
+        <v>0.0688760909635338</v>
+      </c>
+      <c r="H84" s="6" t="n">
         <v>164.286204149886</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="2" t="n">
+      <c r="A85" s="3" t="n">
         <v>43070</v>
       </c>
       <c r="B85" s="0" t="n">
@@ -2489,24 +2497,24 @@
       <c r="C85" s="0" t="n">
         <v>1473.11944444444</v>
       </c>
-      <c r="D85" s="3" t="n">
+      <c r="D85" s="2" t="n">
         <v>4.175</v>
       </c>
-      <c r="E85" s="6" t="n">
+      <c r="E85" s="7" t="n">
         <v>4.09</v>
       </c>
-      <c r="F85" s="0" t="n">
-        <v>4.71641674378703</v>
-      </c>
-      <c r="G85" s="0" t="n">
-        <v>6.75979918840102</v>
-      </c>
-      <c r="H85" s="5" t="n">
+      <c r="F85" s="8" t="n">
+        <v>0.0471641674378703</v>
+      </c>
+      <c r="G85" s="8" t="n">
+        <v>0.0675979918840102</v>
+      </c>
+      <c r="H85" s="6" t="n">
         <v>160.249352775465</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="2" t="n">
+      <c r="A86" s="3" t="n">
         <v>43101</v>
       </c>
       <c r="B86" s="0" t="n">
@@ -2515,24 +2523,24 @@
       <c r="C86" s="0" t="n">
         <v>1551.15142857143</v>
       </c>
-      <c r="D86" s="3" t="n">
+      <c r="D86" s="2" t="n">
         <v>3.407</v>
       </c>
       <c r="E86" s="4" t="n">
         <v>3.68</v>
       </c>
-      <c r="F86" s="0" t="n">
-        <v>4.75133502411786</v>
-      </c>
-      <c r="G86" s="0" t="n">
-        <v>6.69986916949756</v>
-      </c>
-      <c r="H86" s="5" t="n">
+      <c r="F86" s="8" t="n">
+        <v>0.0475133502411786</v>
+      </c>
+      <c r="G86" s="8" t="n">
+        <v>0.0669986916949756</v>
+      </c>
+      <c r="H86" s="6" t="n">
         <v>142.927637031065</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="2" t="n">
+      <c r="A87" s="3" t="n">
         <v>43132</v>
       </c>
       <c r="B87" s="0" t="n">
@@ -2541,24 +2549,24 @@
       <c r="C87" s="0" t="n">
         <v>1522.122</v>
       </c>
-      <c r="D87" s="3" t="n">
+      <c r="D87" s="2" t="n">
         <v>3.55</v>
       </c>
-      <c r="E87" s="6" t="n">
+      <c r="E87" s="7" t="n">
         <v>3.37</v>
       </c>
-      <c r="F87" s="0" t="n">
-        <v>4.79439017753604</v>
-      </c>
-      <c r="G87" s="0" t="n">
-        <v>6.8570823799497</v>
-      </c>
-      <c r="H87" s="5" t="n">
+      <c r="F87" s="8" t="n">
+        <v>0.0479439017753604</v>
+      </c>
+      <c r="G87" s="8" t="n">
+        <v>0.068570823799497</v>
+      </c>
+      <c r="H87" s="6" t="n">
         <v>153.251940401049</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="2" t="n">
+      <c r="A88" s="3" t="n">
         <v>43160</v>
       </c>
       <c r="B88" s="0" t="n">
@@ -2567,24 +2575,24 @@
       <c r="C88" s="0" t="n">
         <v>1469.28421052632</v>
       </c>
-      <c r="D88" s="3" t="n">
+      <c r="D88" s="2" t="n">
         <v>3.5</v>
       </c>
       <c r="E88" s="4" t="n">
         <v>3.14</v>
       </c>
-      <c r="F88" s="0" t="n">
-        <v>4.65062100767898</v>
-      </c>
-      <c r="G88" s="0" t="n">
-        <v>6.9595079809103</v>
-      </c>
-      <c r="H88" s="5" t="n">
+      <c r="F88" s="8" t="n">
+        <v>0.0465062100767898</v>
+      </c>
+      <c r="G88" s="8" t="n">
+        <v>0.069595079809103</v>
+      </c>
+      <c r="H88" s="6" t="n">
         <v>158.751619337855</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="2" t="n">
+      <c r="A89" s="3" t="n">
         <v>43191</v>
       </c>
       <c r="B89" s="0" t="n">
@@ -2593,24 +2601,24 @@
       <c r="C89" s="0" t="n">
         <v>1542.46904761905</v>
       </c>
-      <c r="D89" s="3" t="n">
+      <c r="D89" s="2" t="n">
         <v>3.4</v>
       </c>
-      <c r="E89" s="6" t="n">
+      <c r="E89" s="7" t="n">
         <v>3.13</v>
       </c>
-      <c r="F89" s="0" t="n">
-        <v>4.46901397267114</v>
-      </c>
-      <c r="G89" s="0" t="n">
-        <v>6.66592967114122</v>
-      </c>
-      <c r="H89" s="5" t="n">
+      <c r="F89" s="8" t="n">
+        <v>0.0446901397267114</v>
+      </c>
+      <c r="G89" s="8" t="n">
+        <v>0.0666592967114122</v>
+      </c>
+      <c r="H89" s="6" t="n">
         <v>181.885384341156</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="2" t="n">
+      <c r="A90" s="3" t="n">
         <v>43221</v>
       </c>
       <c r="B90" s="0" t="n">
@@ -2619,24 +2627,24 @@
       <c r="C90" s="0" t="n">
         <v>1540.87142857143</v>
       </c>
-      <c r="D90" s="3" t="n">
+      <c r="D90" s="2" t="n">
         <v>3.55</v>
       </c>
       <c r="E90" s="4" t="n">
         <v>3.16</v>
       </c>
-      <c r="F90" s="0" t="n">
-        <v>4.56487228475955</v>
-      </c>
-      <c r="G90" s="0" t="n">
-        <v>6.82169470048194</v>
-      </c>
-      <c r="H90" s="5" t="n">
+      <c r="F90" s="8" t="n">
+        <v>0.0456487228475955</v>
+      </c>
+      <c r="G90" s="8" t="n">
+        <v>0.0682169470048194</v>
+      </c>
+      <c r="H90" s="6" t="n">
         <v>159.780333187808</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="2" t="n">
+      <c r="A91" s="3" t="n">
         <v>43252</v>
       </c>
       <c r="B91" s="0" t="n">
@@ -2645,24 +2653,24 @@
       <c r="C91" s="0" t="n">
         <v>1547.58105263158</v>
       </c>
-      <c r="D91" s="3" t="n">
+      <c r="D91" s="2" t="n">
         <v>3.5</v>
       </c>
-      <c r="E91" s="6" t="n">
+      <c r="E91" s="7" t="n">
         <v>3.2</v>
       </c>
-      <c r="F91" s="0" t="n">
-        <v>4.66077934836163</v>
-      </c>
-      <c r="G91" s="0" t="n">
-        <v>6.90119191471258</v>
-      </c>
-      <c r="H91" s="5" t="n">
+      <c r="F91" s="8" t="n">
+        <v>0.0466077934836163</v>
+      </c>
+      <c r="G91" s="8" t="n">
+        <v>0.0690119191471258</v>
+      </c>
+      <c r="H91" s="6" t="n">
         <v>155.391928156177</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="2" t="n">
+      <c r="A92" s="3" t="n">
         <v>43282</v>
       </c>
       <c r="B92" s="0" t="n">
@@ -2671,24 +2679,24 @@
       <c r="C92" s="0" t="n">
         <v>1549.5155</v>
       </c>
-      <c r="D92" s="3" t="n">
+      <c r="D92" s="2" t="n">
         <v>3.492</v>
       </c>
       <c r="E92" s="4" t="n">
         <v>3.12</v>
       </c>
-      <c r="F92" s="0" t="n">
-        <v>4.69974988846775</v>
-      </c>
-      <c r="G92" s="0" t="n">
-        <v>6.96566881825426</v>
-      </c>
-      <c r="H92" s="5" t="n">
+      <c r="F92" s="8" t="n">
+        <v>0.0469974988846775</v>
+      </c>
+      <c r="G92" s="8" t="n">
+        <v>0.0696566881825426</v>
+      </c>
+      <c r="H92" s="6" t="n">
         <v>165.920389734011</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="2" t="n">
+      <c r="A93" s="3" t="n">
         <v>43313</v>
       </c>
       <c r="B93" s="0" t="n">
@@ -2697,24 +2705,24 @@
       <c r="C93" s="0" t="n">
         <v>1533.75523809524</v>
       </c>
-      <c r="D93" s="3" t="n">
+      <c r="D93" s="2" t="n">
         <v>3.475</v>
       </c>
-      <c r="E93" s="6" t="n">
+      <c r="E93" s="7" t="n">
         <v>3.1</v>
       </c>
-      <c r="F93" s="0" t="n">
-        <v>4.72629897455842</v>
-      </c>
-      <c r="G93" s="0" t="n">
-        <v>7.10368725888687</v>
-      </c>
-      <c r="H93" s="5" t="n">
+      <c r="F93" s="8" t="n">
+        <v>0.0472629897455842</v>
+      </c>
+      <c r="G93" s="8" t="n">
+        <v>0.0710368725888687</v>
+      </c>
+      <c r="H93" s="6" t="n">
         <v>171.005970074666</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="2" t="n">
+      <c r="A94" s="3" t="n">
         <v>43344</v>
       </c>
       <c r="B94" s="0" t="n">
@@ -2723,24 +2731,24 @@
       <c r="C94" s="0" t="n">
         <v>1497.526</v>
       </c>
-      <c r="D94" s="3" t="n">
+      <c r="D94" s="2" t="n">
         <v>3.48</v>
       </c>
       <c r="E94" s="4" t="n">
         <v>3.23</v>
       </c>
-      <c r="F94" s="0" t="n">
-        <v>4.72695894097999</v>
-      </c>
-      <c r="G94" s="0" t="n">
-        <v>7.15720168731577</v>
-      </c>
-      <c r="H94" s="5" t="n">
+      <c r="F94" s="8" t="n">
+        <v>0.0472695894097999</v>
+      </c>
+      <c r="G94" s="8" t="n">
+        <v>0.0715720168731577</v>
+      </c>
+      <c r="H94" s="6" t="n">
         <v>173.20707434642</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="2" t="n">
+      <c r="A95" s="3" t="n">
         <v>43374</v>
       </c>
       <c r="B95" s="0" t="n">
@@ -2749,24 +2757,24 @@
       <c r="C95" s="0" t="n">
         <v>1457.94227272727</v>
       </c>
-      <c r="D95" s="3" t="n">
+      <c r="D95" s="2" t="n">
         <v>3.41</v>
       </c>
-      <c r="E95" s="6" t="n">
+      <c r="E95" s="7" t="n">
         <v>3.33</v>
       </c>
-      <c r="F95" s="0" t="n">
-        <v>4.79250946727271</v>
-      </c>
-      <c r="G95" s="0" t="n">
-        <v>7.31188279468563</v>
-      </c>
-      <c r="H95" s="5" t="n">
+      <c r="F95" s="8" t="n">
+        <v>0.0479250946727271</v>
+      </c>
+      <c r="G95" s="8" t="n">
+        <v>0.0731188279468563</v>
+      </c>
+      <c r="H95" s="6" t="n">
         <v>169.430087193468</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="2" t="n">
+      <c r="A96" s="3" t="n">
         <v>43405</v>
       </c>
       <c r="B96" s="0" t="n">
@@ -2775,24 +2783,24 @@
       <c r="C96" s="0" t="n">
         <v>1399.322</v>
       </c>
-      <c r="D96" s="3" t="n">
+      <c r="D96" s="2" t="n">
         <v>3.275</v>
       </c>
       <c r="E96" s="4" t="n">
         <v>3.27</v>
       </c>
-      <c r="F96" s="0" t="n">
-        <v>4.88491075028238</v>
-      </c>
-      <c r="G96" s="0" t="n">
-        <v>7.34812908861511</v>
-      </c>
-      <c r="H96" s="5" t="n">
+      <c r="F96" s="8" t="n">
+        <v>0.0488491075028238</v>
+      </c>
+      <c r="G96" s="8" t="n">
+        <v>0.0734812908861511</v>
+      </c>
+      <c r="H96" s="6" t="n">
         <v>171.9624213817</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="2" t="n">
+      <c r="A97" s="3" t="n">
         <v>43435</v>
       </c>
       <c r="B97" s="0" t="n">
@@ -2801,24 +2809,24 @@
       <c r="C97" s="0" t="n">
         <v>1353.76526315789</v>
       </c>
-      <c r="D97" s="3" t="n">
+      <c r="D97" s="2" t="n">
         <v>3.3</v>
       </c>
-      <c r="E97" s="6" t="n">
+      <c r="E97" s="7" t="n">
         <v>3.18</v>
       </c>
-      <c r="F97" s="0" t="n">
-        <v>4.84684673414476</v>
-      </c>
-      <c r="G97" s="0" t="n">
-        <v>7.13311054524496</v>
-      </c>
-      <c r="H97" s="5" t="n">
+      <c r="F97" s="8" t="n">
+        <v>0.0484684673414476</v>
+      </c>
+      <c r="G97" s="8" t="n">
+        <v>0.0713311054524496</v>
+      </c>
+      <c r="H97" s="6" t="n">
         <v>158.948884878707</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="2" t="n">
+      <c r="A98" s="3" t="n">
         <v>43466</v>
       </c>
       <c r="B98" s="0" t="n">
@@ -2827,24 +2835,24 @@
       <c r="C98" s="0" t="n">
         <v>1396.87142857143</v>
       </c>
-      <c r="D98" s="3" t="n">
+      <c r="D98" s="2" t="n">
         <v>3.17</v>
       </c>
       <c r="E98" s="4" t="n">
         <v>3.15</v>
       </c>
-      <c r="F98" s="0" t="n">
-        <v>4.84435666909759</v>
-      </c>
-      <c r="G98" s="0" t="n">
-        <v>7.06539018824607</v>
-      </c>
-      <c r="H98" s="5" t="n">
+      <c r="F98" s="8" t="n">
+        <v>0.0484435666909759</v>
+      </c>
+      <c r="G98" s="8" t="n">
+        <v>0.0706539018824607</v>
+      </c>
+      <c r="H98" s="6" t="n">
         <v>146.910453443072</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="2" t="n">
+      <c r="A99" s="3" t="n">
         <v>43497</v>
       </c>
       <c r="B99" s="0" t="n">
@@ -2853,24 +2861,24 @@
       <c r="C99" s="0" t="n">
         <v>1485.2275</v>
       </c>
-      <c r="D99" s="3" t="n">
+      <c r="D99" s="2" t="n">
         <v>3.225</v>
       </c>
-      <c r="E99" s="6" t="n">
+      <c r="E99" s="7" t="n">
         <v>3.01</v>
       </c>
-      <c r="F99" s="0" t="n">
-        <v>4.75992938797435</v>
-      </c>
-      <c r="G99" s="0" t="n">
-        <v>6.975901945806</v>
-      </c>
-      <c r="H99" s="5" t="n">
+      <c r="F99" s="8" t="n">
+        <v>0.0475992938797435</v>
+      </c>
+      <c r="G99" s="8" t="n">
+        <v>0.06975901945806</v>
+      </c>
+      <c r="H99" s="6" t="n">
         <v>157.689542074208</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="2" t="n">
+      <c r="A100" s="3" t="n">
         <v>43525</v>
       </c>
       <c r="B100" s="0" t="n">
@@ -2879,24 +2887,24 @@
       <c r="C100" s="0" t="n">
         <v>1564.5995</v>
       </c>
-      <c r="D100" s="3" t="n">
+      <c r="D100" s="2" t="n">
         <v>3.2</v>
       </c>
       <c r="E100" s="4" t="n">
         <v>3.21</v>
       </c>
-      <c r="F100" s="0" t="n">
-        <v>4.62245423887107</v>
-      </c>
-      <c r="G100" s="0" t="n">
-        <v>6.83471925934587</v>
-      </c>
-      <c r="H100" s="5" t="n">
+      <c r="F100" s="8" t="n">
+        <v>0.0462245423887107</v>
+      </c>
+      <c r="G100" s="8" t="n">
+        <v>0.0683471925934587</v>
+      </c>
+      <c r="H100" s="6" t="n">
         <v>163.452782690122</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="2" t="n">
+      <c r="A101" s="3" t="n">
         <v>43556</v>
       </c>
       <c r="B101" s="0" t="n">
@@ -2905,24 +2913,24 @@
       <c r="C101" s="0" t="n">
         <v>1594.9</v>
       </c>
-      <c r="D101" s="3" t="n">
+      <c r="D101" s="2" t="n">
         <v>3.32</v>
       </c>
-      <c r="E101" s="6" t="n">
+      <c r="E101" s="7" t="n">
         <v>3.25</v>
       </c>
-      <c r="F101" s="0" t="n">
-        <v>4.58470514618347</v>
-      </c>
-      <c r="G101" s="0" t="n">
-        <v>6.75904569205578</v>
-      </c>
-      <c r="H101" s="5" t="n">
+      <c r="F101" s="8" t="n">
+        <v>0.0458470514618347</v>
+      </c>
+      <c r="G101" s="8" t="n">
+        <v>0.0675904569205578</v>
+      </c>
+      <c r="H101" s="6" t="n">
         <v>179.185536058052</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="2" t="n">
+      <c r="A102" s="3" t="n">
         <v>43586</v>
       </c>
       <c r="B102" s="0" t="n">
@@ -2931,24 +2939,24 @@
       <c r="C102" s="0" t="n">
         <v>1508.635</v>
       </c>
-      <c r="D102" s="3" t="n">
+      <c r="D102" s="2" t="n">
         <v>3.225</v>
       </c>
       <c r="E102" s="4" t="n">
         <v>3.31</v>
       </c>
-      <c r="F102" s="0" t="n">
-        <v>4.59988616166087</v>
-      </c>
-      <c r="G102" s="0" t="n">
-        <v>6.88138636557612</v>
-      </c>
-      <c r="H102" s="5" t="n">
+      <c r="F102" s="8" t="n">
+        <v>0.0459988616166087</v>
+      </c>
+      <c r="G102" s="8" t="n">
+        <v>0.0688138636557612</v>
+      </c>
+      <c r="H102" s="6" t="n">
         <v>165.302696667488</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="2" t="n">
+      <c r="A103" s="3" t="n">
         <v>43617</v>
       </c>
       <c r="B103" s="0" t="n">
@@ -2957,24 +2965,24 @@
       <c r="C103" s="0" t="n">
         <v>1526.79833333333</v>
       </c>
-      <c r="D103" s="3" t="n">
+      <c r="D103" s="2" t="n">
         <v>3.3</v>
       </c>
-      <c r="E103" s="6" t="n">
+      <c r="E103" s="7" t="n">
         <v>3.43</v>
       </c>
-      <c r="F103" s="0" t="n">
-        <v>4.39269981348228</v>
-      </c>
-      <c r="G103" s="0" t="n">
-        <v>6.40339664827428</v>
-      </c>
-      <c r="H103" s="5" t="n">
+      <c r="F103" s="8" t="n">
+        <v>0.0439269981348228</v>
+      </c>
+      <c r="G103" s="8" t="n">
+        <v>0.0640339664827428</v>
+      </c>
+      <c r="H103" s="6" t="n">
         <v>153.907906764364</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="2" t="n">
+      <c r="A104" s="3" t="n">
         <v>43647</v>
       </c>
       <c r="B104" s="0" t="n">
@@ -2983,24 +2991,24 @@
       <c r="C104" s="0" t="n">
         <v>1587.68909090909</v>
       </c>
-      <c r="D104" s="3" t="n">
+      <c r="D104" s="2" t="n">
         <v>3.347</v>
       </c>
       <c r="E104" s="4" t="n">
         <v>3.79</v>
       </c>
-      <c r="F104" s="0" t="n">
-        <v>4.33923735753062</v>
-      </c>
-      <c r="G104" s="0" t="n">
-        <v>6.05999115777623</v>
-      </c>
-      <c r="H104" s="5" t="n">
+      <c r="F104" s="8" t="n">
+        <v>0.0433923735753062</v>
+      </c>
+      <c r="G104" s="8" t="n">
+        <v>0.0605999115777623</v>
+      </c>
+      <c r="H104" s="6" t="n">
         <v>172.06100103402</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="2" t="n">
+      <c r="A105" s="3" t="n">
         <v>43678</v>
       </c>
       <c r="B105" s="0" t="n">
@@ -3009,24 +3017,24 @@
       <c r="C105" s="0" t="n">
         <v>1533.0025</v>
       </c>
-      <c r="D105" s="3" t="n">
+      <c r="D105" s="2" t="n">
         <v>3.225</v>
       </c>
-      <c r="E105" s="6" t="n">
+      <c r="E105" s="7" t="n">
         <v>3.75</v>
       </c>
-      <c r="F105" s="0" t="n">
-        <v>4.46411233177918</v>
-      </c>
-      <c r="G105" s="0" t="n">
-        <v>6.0786759111026</v>
-      </c>
-      <c r="H105" s="5" t="n">
+      <c r="F105" s="8" t="n">
+        <v>0.0446411233177918</v>
+      </c>
+      <c r="G105" s="8" t="n">
+        <v>0.060786759111026</v>
+      </c>
+      <c r="H105" s="6" t="n">
         <v>171.471000139232</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="2" t="n">
+      <c r="A106" s="3" t="n">
         <v>43709</v>
       </c>
       <c r="B106" s="0" t="n">
@@ -3035,24 +3043,24 @@
       <c r="C106" s="0" t="n">
         <v>1583.80142857143</v>
       </c>
-      <c r="D106" s="3" t="n">
+      <c r="D106" s="2" t="n">
         <v>3.3</v>
       </c>
       <c r="E106" s="4" t="n">
         <v>3.82</v>
       </c>
-      <c r="F106" s="0" t="n">
-        <v>4.42651585420406</v>
-      </c>
-      <c r="G106" s="0" t="n">
-        <v>6.10025221895612</v>
-      </c>
-      <c r="H106" s="5" t="n">
+      <c r="F106" s="8" t="n">
+        <v>0.0442651585420406</v>
+      </c>
+      <c r="G106" s="8" t="n">
+        <v>0.0610025221895612</v>
+      </c>
+      <c r="H106" s="6" t="n">
         <v>174.038345566359</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="2" t="n">
+      <c r="A107" s="3" t="n">
         <v>43739</v>
       </c>
       <c r="B107" s="0" t="n">
@@ -3061,24 +3069,24 @@
       <c r="C107" s="0" t="n">
         <v>1599.82954545455</v>
       </c>
-      <c r="D107" s="3" t="n">
+      <c r="D107" s="2" t="n">
         <v>3.523</v>
       </c>
-      <c r="E107" s="6" t="n">
+      <c r="E107" s="7" t="n">
         <v>3.86</v>
       </c>
-      <c r="F107" s="0" t="n">
-        <v>4.47427246338372</v>
-      </c>
-      <c r="G107" s="0" t="n">
-        <v>6.10390515793094</v>
-      </c>
-      <c r="H107" s="5" t="n">
+      <c r="F107" s="8" t="n">
+        <v>0.0447427246338372</v>
+      </c>
+      <c r="G107" s="8" t="n">
+        <v>0.0610390515793094</v>
+      </c>
+      <c r="H107" s="6" t="n">
         <v>173.122271531086</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="2" t="n">
+      <c r="A108" s="3" t="n">
         <v>43770</v>
       </c>
       <c r="B108" s="0" t="n">
@@ -3087,24 +3095,24 @@
       <c r="C108" s="0" t="n">
         <v>1621.64157894737</v>
       </c>
-      <c r="D108" s="3" t="n">
+      <c r="D108" s="2" t="n">
         <v>3.566</v>
       </c>
       <c r="E108" s="4" t="n">
         <v>3.84</v>
       </c>
-      <c r="F108" s="0" t="n">
-        <v>4.60439548997421</v>
-      </c>
-      <c r="G108" s="0" t="n">
-        <v>6.40603399889046</v>
-      </c>
-      <c r="H108" s="5" t="n">
+      <c r="F108" s="8" t="n">
+        <v>0.0460439548997421</v>
+      </c>
+      <c r="G108" s="8" t="n">
+        <v>0.0640603399889046</v>
+      </c>
+      <c r="H108" s="6" t="n">
         <v>168.481505428179</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="2" t="n">
+      <c r="A109" s="3" t="n">
         <v>43800</v>
       </c>
       <c r="B109" s="0" t="n">
@@ -3113,19 +3121,19 @@
       <c r="C109" s="0" t="n">
         <v>1629.3615</v>
       </c>
-      <c r="D109" s="3" t="n">
+      <c r="D109" s="2" t="n">
         <v>3.534</v>
       </c>
-      <c r="E109" s="6" t="n">
+      <c r="E109" s="7" t="n">
         <v>3.8</v>
       </c>
-      <c r="F109" s="0" t="n">
-        <v>4.55869965516408</v>
-      </c>
-      <c r="G109" s="0" t="n">
-        <v>6.40941508563821</v>
-      </c>
-      <c r="H109" s="5" t="n">
+      <c r="F109" s="8" t="n">
+        <v>0.0455869965516408</v>
+      </c>
+      <c r="G109" s="8" t="n">
+        <v>0.0640941508563821</v>
+      </c>
+      <c r="H109" s="6" t="n">
         <v>164.379241142677</v>
       </c>
     </row>

</xml_diff>